<commit_message>
Batterij circuit beslissing genomen
Beslissing genomen over het oplaad IC, protectie IC, dual N-ch mosfets, batterij. BOM aangepast me 3 verschillende sites bij (farnell, digi-key en mouser). + IC's geplaatst in MainPCB
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\GitHub\cosy_cafeteria\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\Documents\GitHub\cosy_cafeteria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E68DF04-3168-4FF8-B70B-D7E3681675DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8AABDB-7CB2-4F72-AA38-F7D73E3D015F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>Part No.</t>
   </si>
@@ -33,24 +33,9 @@
     <t>Description</t>
   </si>
   <si>
-    <t>FS8205A</t>
-  </si>
-  <si>
-    <t>Dual MOSFET 8205A</t>
-  </si>
-  <si>
     <t>Function</t>
   </si>
   <si>
-    <t>Charge circuit 3,7V lithium-ion ion battery</t>
-  </si>
-  <si>
-    <t>BQ24004</t>
-  </si>
-  <si>
-    <t>Charger chip + protection</t>
-  </si>
-  <si>
     <t xml:space="preserve">Wi-Fi module: </t>
   </si>
   <si>
@@ -64,13 +49,115 @@
   </si>
   <si>
     <t xml:space="preserve"> DEBO ESP8266-12F</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>Charger chip</t>
+  </si>
+  <si>
+    <t>Protection IC</t>
+  </si>
+  <si>
+    <t>https://www.tinytronics.nl/shop/nl/batterij-en-accu/18650/panasonic-18650-li-ion-batterij-3350mah-6.7a-ncr18650b?fbclid=IwAR0iy0AZsec7F5R9p64jz5AuVEGUysugrAmQHkZzPpcWrmf20fGhfmFC5nM</t>
+  </si>
+  <si>
+    <t>18650 Li-ion Batterij, 3350mAh</t>
+  </si>
+  <si>
+    <t>NCR18650B</t>
+  </si>
+  <si>
+    <t>Battery holder</t>
+  </si>
+  <si>
+    <t>https://www.digikey.be/product-detail/nl/keystone-electronics/1043/36-1043-ND/2745669</t>
+  </si>
+  <si>
+    <t>BATTERY HOLDER 18650 PC PIN</t>
+  </si>
+  <si>
+    <t>‎36-1043-ND‎</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/keystone/1043p/battery-holder-18650-th/dp/2673609</t>
+  </si>
+  <si>
+    <t>Prijs</t>
+  </si>
+  <si>
+    <t>Charge circuit 3,7V lithium ion battery</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/texas-instruments/bq29700dset/batt-prot-li-ion-li-pol-4-275v/dp/3123826?st=BQ29700</t>
+  </si>
+  <si>
+    <t>BQ29700DSET</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>WSON-6</t>
+  </si>
+  <si>
+    <t>BQ29700DSER</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Texas-Instruments/BQ29700DSER?qs=sGAEpiMZZMtp5ziQ9mm%252BAtGylTWQnXFkISzO83o5y%252B0%3D</t>
+  </si>
+  <si>
+    <t>BQ24075RGTR</t>
+  </si>
+  <si>
+    <t>VQFN-16</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Texas-Instruments/BQ24075RGTR?qs=sGAEpiMZZMsfD%252BbMpEGFJacQ2ERStaA380DS33yrLsc%3D</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/texas-instruments/bq24075rgtr/batt-charger-li-ion-1-5a-vqfn/dp/3123776?st=BQ24075</t>
+  </si>
+  <si>
+    <t>https://www.digikey.be/product-detail/nl/texas-instruments/BQ24075RGTR/296-38874-1-ND/5142986</t>
+  </si>
+  <si>
+    <t>https://www.digikey.be/product-detail/nl/texas-instruments/BQ29700DSER/296-43985-1-ND/5973209</t>
+  </si>
+  <si>
+    <t>https://www.digikey.be/product-detail/nl/on-semiconductor/FDS9926A/FDS9926ACT-ND/965635</t>
+  </si>
+  <si>
+    <t>8-SOIC</t>
+  </si>
+  <si>
+    <t>FDS9926ACT-ND</t>
+  </si>
+  <si>
+    <t>FDS9926A</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/on-semiconductor/fds9926a/mosfet-dual-n-smd-so-8/dp/1467990?st=FDS9926A</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/ON-Semiconductor-Fairchild/FDS9926A?qs=%2Fha2pyFaduiTKNA0VGG3ImYYElJw72OjoEu%2FUJRB%2Flc%3D</t>
+  </si>
+  <si>
+    <t>512-FDS9926A</t>
+  </si>
+  <si>
+    <t>Dual N-channel MOSFETs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +177,18 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,20 +224,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -420,24 +533,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="220.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="34.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="30" style="5" customWidth="1"/>
+    <col min="3" max="4" width="18.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="220.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="4" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -445,48 +559,262 @@
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="9">
+        <v>1.85</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="9">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="9">
+        <v>1.99</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0.66</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0.51</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0.51</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0.54</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="9">
+        <v>4.95</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="9">
+        <v>2.34</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>10</v>
-      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="9"/>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="9"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" xr:uid="{8B37AF3C-3179-401B-9F44-E094BA43E056}"/>
+    <hyperlink ref="F14" r:id="rId1" xr:uid="{8B37AF3C-3179-401B-9F44-E094BA43E056}"/>
+    <hyperlink ref="F11" r:id="rId2" xr:uid="{BE201204-4D76-4D99-A136-97852DAF4D35}"/>
+    <hyperlink ref="F13" r:id="rId3" xr:uid="{A163CA04-1225-4998-8A7A-0977D492F5D7}"/>
+    <hyperlink ref="F12" r:id="rId4" xr:uid="{4F87FBD2-AD24-4856-A19A-6D777E589112}"/>
+    <hyperlink ref="F5" r:id="rId5" xr:uid="{DC8C48DE-7270-47F8-B3DF-2C4BDE7D1D0A}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{C67E4CED-6F3A-4EC3-A9D8-987FB4B57235}"/>
+    <hyperlink ref="F4" r:id="rId7" xr:uid="{581F1366-C05C-44C0-8730-D2774468FBE7}"/>
+    <hyperlink ref="F2" r:id="rId8" xr:uid="{736606E3-F482-4B9A-9F8A-6DA9174AF1D7}"/>
+    <hyperlink ref="F3" r:id="rId9" xr:uid="{BB5014F1-E9FC-4992-AEC5-4AECDBABD85E}"/>
+    <hyperlink ref="F6" r:id="rId10" xr:uid="{CF21DD32-9D2B-45E5-B62C-FF494374B6FC}"/>
+    <hyperlink ref="F9" r:id="rId11" xr:uid="{9EF89D16-1463-4389-A813-66591B5D9D72}"/>
+    <hyperlink ref="F8" r:id="rId12" xr:uid="{B665DE4A-E4CF-4C23-90A3-80D7A24101EA}"/>
+    <hyperlink ref="F10" r:id="rId13" xr:uid="{AFCDD530-6064-45FD-891D-CCEADAF8BFA1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed battery holder 1043 TH to 1042 SMD
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\Documents\GitHub\cosy_cafeteria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8AABDB-7CB2-4F72-AA38-F7D73E3D015F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3FE384-85E1-4B62-A8A0-28711E23A6E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>Part No.</t>
   </si>
@@ -78,12 +78,6 @@
     <t>BATTERY HOLDER 18650 PC PIN</t>
   </si>
   <si>
-    <t>‎36-1043-ND‎</t>
-  </si>
-  <si>
-    <t>https://be.farnell.com/keystone/1043p/battery-holder-18650-th/dp/2673609</t>
-  </si>
-  <si>
     <t>Prijs</t>
   </si>
   <si>
@@ -148,6 +142,18 @@
   </si>
   <si>
     <t>Dual N-channel MOSFETs</t>
+  </si>
+  <si>
+    <t>2,2+25 zendkosten</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/keystone/1042p/battery-holder-18650-smd/dp/2674338?ost=keystone+1042&amp;cfm=true&amp;ddkey=https%3Anl-BE%2FElement14_Belgium%2Fsearch</t>
+  </si>
+  <si>
+    <t>36-1042P-ND</t>
+  </si>
+  <si>
+    <t>battery is too expensive on farnell and digi-key (30 euro)</t>
   </si>
 </sst>
 </file>
@@ -533,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,10 +566,10 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>6</v>
@@ -571,50 +577,50 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E2" s="9">
         <v>1.85</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E3" s="9">
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E4" s="9">
         <v>1.99</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -622,89 +628,89 @@
         <v>10</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>24</v>
       </c>
       <c r="E5" s="9">
         <v>0.66</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E6" s="9">
         <v>0.56000000000000005</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C7" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E7" s="9">
         <v>0.6</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E8" s="9">
         <v>0.51</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E9" s="9">
         <v>0.51</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E10" s="9">
         <v>0.54</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -725,47 +731,50 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="E12" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="9">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E13" s="9">
-        <v>2.34</v>
-      </c>
-      <c r="F13" s="6" t="s">
+      <c r="E13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="9">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="8" t="s">
+      <c r="E15" s="9"/>
+      <c r="F15" s="8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E16" s="9"/>
@@ -796,25 +805,29 @@
     </row>
     <row r="25" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E25" s="9"/>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F14" r:id="rId1" xr:uid="{8B37AF3C-3179-401B-9F44-E094BA43E056}"/>
+    <hyperlink ref="F15" r:id="rId1" xr:uid="{8B37AF3C-3179-401B-9F44-E094BA43E056}"/>
     <hyperlink ref="F11" r:id="rId2" xr:uid="{BE201204-4D76-4D99-A136-97852DAF4D35}"/>
-    <hyperlink ref="F13" r:id="rId3" xr:uid="{A163CA04-1225-4998-8A7A-0977D492F5D7}"/>
-    <hyperlink ref="F12" r:id="rId4" xr:uid="{4F87FBD2-AD24-4856-A19A-6D777E589112}"/>
-    <hyperlink ref="F5" r:id="rId5" xr:uid="{DC8C48DE-7270-47F8-B3DF-2C4BDE7D1D0A}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{C67E4CED-6F3A-4EC3-A9D8-987FB4B57235}"/>
-    <hyperlink ref="F4" r:id="rId7" xr:uid="{581F1366-C05C-44C0-8730-D2774468FBE7}"/>
-    <hyperlink ref="F2" r:id="rId8" xr:uid="{736606E3-F482-4B9A-9F8A-6DA9174AF1D7}"/>
-    <hyperlink ref="F3" r:id="rId9" xr:uid="{BB5014F1-E9FC-4992-AEC5-4AECDBABD85E}"/>
-    <hyperlink ref="F6" r:id="rId10" xr:uid="{CF21DD32-9D2B-45E5-B62C-FF494374B6FC}"/>
-    <hyperlink ref="F9" r:id="rId11" xr:uid="{9EF89D16-1463-4389-A813-66591B5D9D72}"/>
-    <hyperlink ref="F8" r:id="rId12" xr:uid="{B665DE4A-E4CF-4C23-90A3-80D7A24101EA}"/>
-    <hyperlink ref="F10" r:id="rId13" xr:uid="{AFCDD530-6064-45FD-891D-CCEADAF8BFA1}"/>
+    <hyperlink ref="F14" r:id="rId3" xr:uid="{A163CA04-1225-4998-8A7A-0977D492F5D7}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{DC8C48DE-7270-47F8-B3DF-2C4BDE7D1D0A}"/>
+    <hyperlink ref="F7" r:id="rId5" xr:uid="{C67E4CED-6F3A-4EC3-A9D8-987FB4B57235}"/>
+    <hyperlink ref="F4" r:id="rId6" xr:uid="{581F1366-C05C-44C0-8730-D2774468FBE7}"/>
+    <hyperlink ref="F2" r:id="rId7" xr:uid="{736606E3-F482-4B9A-9F8A-6DA9174AF1D7}"/>
+    <hyperlink ref="F3" r:id="rId8" xr:uid="{BB5014F1-E9FC-4992-AEC5-4AECDBABD85E}"/>
+    <hyperlink ref="F6" r:id="rId9" xr:uid="{CF21DD32-9D2B-45E5-B62C-FF494374B6FC}"/>
+    <hyperlink ref="F9" r:id="rId10" xr:uid="{9EF89D16-1463-4389-A813-66591B5D9D72}"/>
+    <hyperlink ref="F8" r:id="rId11" xr:uid="{B665DE4A-E4CF-4C23-90A3-80D7A24101EA}"/>
+    <hyperlink ref="F10" r:id="rId12" xr:uid="{AFCDD530-6064-45FD-891D-CCEADAF8BFA1}"/>
+    <hyperlink ref="F13" r:id="rId13" xr:uid="{445D5282-39EA-4E3B-897E-1BE4D1BB3121}"/>
+    <hyperlink ref="C14" r:id="rId14" display="https://www.digikey.be/product-detail/nl/keystone-electronics/1042P/36-1042P-ND/4286267" xr:uid="{6DB4781A-56A7-43A7-99D6-DA10845E2272}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update BOM. Only Mouser links
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gebruikersnaam\Documents\GitHub\cosy_cafeteria\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\Documents\GitHub\cosy_cafeteria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF15EAC7-9DEA-4CFA-BF64-932D44372EBB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6EA2F8-79AE-4AB3-AE91-A39C43D20821}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t>Part No.</t>
   </si>
@@ -79,21 +79,12 @@
     <t>Battery holder</t>
   </si>
   <si>
-    <t>https://www.digikey.be/product-detail/nl/keystone-electronics/1043/36-1043-ND/2745669</t>
-  </si>
-  <si>
     <t>BATTERY HOLDER 18650 PC PIN</t>
   </si>
   <si>
     <t>Prijs</t>
   </si>
   <si>
-    <t>https://be.farnell.com/texas-instruments/bq29700dset/batt-prot-li-ion-li-pol-4-275v/dp/3123826?st=BQ29700</t>
-  </si>
-  <si>
-    <t>BQ29700DSET</t>
-  </si>
-  <si>
     <t>Package</t>
   </si>
   <si>
@@ -115,30 +106,9 @@
     <t>https://www.mouser.be/ProductDetail/Texas-Instruments/BQ24075RGTR?qs=sGAEpiMZZMsfD%252BbMpEGFJacQ2ERStaA380DS33yrLsc%3D</t>
   </si>
   <si>
-    <t>https://be.farnell.com/texas-instruments/bq24075rgtr/batt-charger-li-ion-1-5a-vqfn/dp/3123776?st=BQ24075</t>
-  </si>
-  <si>
-    <t>https://www.digikey.be/product-detail/nl/texas-instruments/BQ24075RGTR/296-38874-1-ND/5142986</t>
-  </si>
-  <si>
-    <t>https://www.digikey.be/product-detail/nl/texas-instruments/BQ29700DSER/296-43985-1-ND/5973209</t>
-  </si>
-  <si>
-    <t>https://www.digikey.be/product-detail/nl/on-semiconductor/FDS9926A/FDS9926ACT-ND/965635</t>
-  </si>
-  <si>
     <t>8-SOIC</t>
   </si>
   <si>
-    <t>FDS9926ACT-ND</t>
-  </si>
-  <si>
-    <t>FDS9926A</t>
-  </si>
-  <si>
-    <t>https://be.farnell.com/on-semiconductor/fds9926a/mosfet-dual-n-smd-so-8/dp/1467990?st=FDS9926A</t>
-  </si>
-  <si>
     <t>https://www.mouser.be/ProductDetail/ON-Semiconductor-Fairchild/FDS9926A?qs=%2Fha2pyFaduiTKNA0VGG3ImYYElJw72OjoEu%2FUJRB%2Flc%3D</t>
   </si>
   <si>
@@ -148,15 +118,6 @@
     <t>Dual N-channel MOSFETs</t>
   </si>
   <si>
-    <t>2,2+25 zendkosten</t>
-  </si>
-  <si>
-    <t>https://be.farnell.com/keystone/1042p/battery-holder-18650-smd/dp/2674338?ost=keystone+1042&amp;cfm=true&amp;ddkey=https%3Anl-BE%2FElement14_Belgium%2Fsearch</t>
-  </si>
-  <si>
-    <t>36-1042P-ND</t>
-  </si>
-  <si>
     <t>battery is too expensive on farnell and digi-key (30 euro)</t>
   </si>
   <si>
@@ -172,15 +133,9 @@
     <t>LDO 3,3V 500 mA</t>
   </si>
   <si>
-    <t>https://www.digikey.be/product-detail/en/texas-instruments/TLV75533PDBVR/296-50411-1-ND/9685550?_ga=2.98561375.1508279743.1582896441-219618250.1582896441</t>
-  </si>
-  <si>
     <t>https://www.mouser.be/ProductDetail/Texas-Instruments/TLV75533PDBVR?qs=sGAEpiMZZMsGz1a6aV8DcD1rpA6FsR3JKgt9d%252BpuSX4%3D</t>
   </si>
   <si>
-    <t>FARNELL DOESN'T HAVE THIS PRODUCT</t>
-  </si>
-  <si>
     <t>534-1042P</t>
   </si>
   <si>
@@ -190,9 +145,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Beste is om op digi-key te bestellen. Bvb: de batterij houder is veel duurder op farnell vanwege amerikaanse stok en de LDO is niet eens verkrijgbaar op farnell. De batterij zelf is het goedkoopst op tinytronics.</t>
-  </si>
-  <si>
     <t>Microfoon</t>
   </si>
   <si>
@@ -232,12 +184,6 @@
     <t>Eval bord</t>
   </si>
   <si>
-    <t>https://www.digikey.be/product-detail/en/sparkfun-electronics/BOB-12758/1568-1472-ND/6592307</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 	BOB-12758</t>
-  </si>
-  <si>
     <t>https://www.mouser.be/Search/Refine?Keyword=AMG8833</t>
   </si>
   <si>
@@ -266,6 +212,12 @@
   </si>
   <si>
     <t>https://www.mouser.be/ProductDetail/ROHM-Semiconductor/RB081LAM-20TR?qs=sGAEpiMZZMtQ8nqTKtFS%2FBUuz6Zx2fl0GeUE2dUwRLrhEAxqSQT8Dw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/SparkFun/BOB-12758?qs=%2Fha2pyFadujP62fbj7HsTYK9R02Dqj4bjucQVz2IrmwHn8AlusFw%252BQ%3D%3D</t>
+  </si>
+  <si>
+    <t>BOB-12758</t>
   </si>
 </sst>
 </file>
@@ -348,7 +300,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -380,9 +332,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -664,55 +613,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S34"/>
+  <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="4" customWidth="1"/>
     <col min="2" max="2" width="29" style="4" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="220.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="4"/>
+    <col min="3" max="3" width="18.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="220.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="10" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-    </row>
-    <row r="2" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+    </row>
+    <row r="2" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8">
+        <v>4.95</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -727,26 +699,16 @@
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
     </row>
-    <row r="3" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>13</v>
-      </c>
+    <row r="3" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="8">
-        <v>4.95</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="F3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="5"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -760,16 +722,26 @@
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
     </row>
-    <row r="4" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+    <row r="4" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" s="5"/>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8">
+        <v>2.17</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -783,23 +755,27 @@
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
     </row>
-    <row r="5" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="8" t="s">
-        <v>38</v>
+        <v>9</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1.99</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -814,19 +790,25 @@
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
     </row>
-    <row r="6" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="D6" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
       <c r="F6" s="8">
-        <v>2.5099999999999998</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>15</v>
+        <v>0.6</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -841,380 +823,204 @@
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
     </row>
-    <row r="7" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="9" t="s">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.54</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="8">
-        <v>2.17</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
+      <c r="F9" s="8">
+        <v>6.26</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" s="8">
+        <v>10.17</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+      <c r="F11" s="8">
+        <v>27.04</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="4">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="8">
-        <v>1.85</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="8">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="8">
-        <v>1.99</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="4">
-        <v>1</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="8">
-        <v>0.66</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>21</v>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1</v>
       </c>
       <c r="F12" s="8">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D13" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>21</v>
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1</v>
       </c>
       <c r="F13" s="8">
-        <v>0.6</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="4">
-        <v>1</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="8">
-        <v>0.51</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="8">
-        <v>0.51</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D16" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="8">
-        <v>0.54</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="4">
-        <v>1</v>
-      </c>
+        <v>5.34</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="9"/>
       <c r="F17" s="8"/>
-      <c r="G17" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D18" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" s="8">
-        <v>0.54</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D19" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="8">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="4">
-        <v>1</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="4">
-        <v>1</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F21" s="8">
-        <v>6.31</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="4">
-        <v>1</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" s="8">
-        <v>10.17</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" s="4">
-        <v>1</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F23" s="8">
-        <v>27.04</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" s="4">
-        <v>1</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F24" s="8">
-        <v>0.35099999999999998</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G17" s="1"/>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F34" s="8"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G20" r:id="rId1" xr:uid="{8B37AF3C-3179-401B-9F44-E094BA43E056}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{BE201204-4D76-4D99-A136-97852DAF4D35}"/>
-    <hyperlink ref="G6" r:id="rId3" xr:uid="{A163CA04-1225-4998-8A7A-0977D492F5D7}"/>
-    <hyperlink ref="G13" r:id="rId4" xr:uid="{C67E4CED-6F3A-4EC3-A9D8-987FB4B57235}"/>
-    <hyperlink ref="G10" r:id="rId5" xr:uid="{581F1366-C05C-44C0-8730-D2774468FBE7}"/>
-    <hyperlink ref="G9" r:id="rId6" xr:uid="{BB5014F1-E9FC-4992-AEC5-4AECDBABD85E}"/>
-    <hyperlink ref="G12" r:id="rId7" xr:uid="{CF21DD32-9D2B-45E5-B62C-FF494374B6FC}"/>
-    <hyperlink ref="G15" r:id="rId8" xr:uid="{9EF89D16-1463-4389-A813-66591B5D9D72}"/>
-    <hyperlink ref="G16" r:id="rId9" xr:uid="{AFCDD530-6064-45FD-891D-CCEADAF8BFA1}"/>
-    <hyperlink ref="G18" r:id="rId10" xr:uid="{79565D10-AEF2-47CD-A765-0C896A168B6D}"/>
-    <hyperlink ref="G19" r:id="rId11" xr:uid="{96DFE09D-FE4D-4147-A8CE-602A5DDFBFA7}"/>
-    <hyperlink ref="G7" r:id="rId12" xr:uid="{682E6110-B477-43CD-9147-49CEB11861DF}"/>
-    <hyperlink ref="G14" r:id="rId13" xr:uid="{B665DE4A-E4CF-4C23-90A3-80D7A24101EA}"/>
-    <hyperlink ref="G11" r:id="rId14" xr:uid="{DC8C48DE-7270-47F8-B3DF-2C4BDE7D1D0A}"/>
-    <hyperlink ref="G8" r:id="rId15" xr:uid="{736606E3-F482-4B9A-9F8A-6DA9174AF1D7}"/>
-    <hyperlink ref="G5" r:id="rId16" xr:uid="{445D5282-39EA-4E3B-897E-1BE4D1BB3121}"/>
-    <hyperlink ref="G24" r:id="rId17" xr:uid="{426BD05D-D8EF-43D7-A582-AC4F8E600E5F}"/>
+    <hyperlink ref="G13" r:id="rId1" xr:uid="{8B37AF3C-3179-401B-9F44-E094BA43E056}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{BE201204-4D76-4D99-A136-97852DAF4D35}"/>
+    <hyperlink ref="G6" r:id="rId3" xr:uid="{C67E4CED-6F3A-4EC3-A9D8-987FB4B57235}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{581F1366-C05C-44C0-8730-D2774468FBE7}"/>
+    <hyperlink ref="G7" r:id="rId5" xr:uid="{AFCDD530-6064-45FD-891D-CCEADAF8BFA1}"/>
+    <hyperlink ref="G8" r:id="rId6" xr:uid="{96DFE09D-FE4D-4147-A8CE-602A5DDFBFA7}"/>
+    <hyperlink ref="G4" r:id="rId7" xr:uid="{682E6110-B477-43CD-9147-49CEB11861DF}"/>
+    <hyperlink ref="G12" r:id="rId8" xr:uid="{426BD05D-D8EF-43D7-A582-AC4F8E600E5F}"/>
+    <hyperlink ref="G10" r:id="rId9" xr:uid="{6E401E59-3667-4D7F-ABA4-4D7A0A7A91E1}"/>
+    <hyperlink ref="G11" r:id="rId10" xr:uid="{340F4965-1516-4699-A1F1-2E724698C5D3}"/>
+    <hyperlink ref="G9" r:id="rId11" xr:uid="{25D5091F-FD09-4C85-B205-63FAF399144A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId12"/>
 </worksheet>
 </file>
 
@@ -1226,49 +1032,49 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="B1" s="4">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="E1" s="8">
         <v>0.70199999999999996</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="E2" s="8">
         <v>0.70199999999999996</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
toevoeging 2x batterijen BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gebruikersnaam\Documents\GitHub\cosy_cafeteria\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\Documents\GitHub\cosy_cafeteria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50598C6-43AE-4162-B6CA-E0A68998B5AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16E35E1-F580-462B-A6B1-ABD7EDDFD549}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -631,22 +631,22 @@
   <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="4" customWidth="1"/>
     <col min="2" max="2" width="29" style="4" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="220.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="4"/>
+    <col min="3" max="3" width="18.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="220.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -681,7 +681,7 @@
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
     </row>
-    <row r="2" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -693,7 +693,7 @@
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" s="8">
         <v>4.95</v>
@@ -714,7 +714,7 @@
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
     </row>
-    <row r="3" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -737,7 +737,7 @@
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
     </row>
-    <row r="4" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -749,7 +749,7 @@
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" s="8">
         <v>2.17</v>
@@ -770,7 +770,7 @@
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
     </row>
-    <row r="5" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -805,7 +805,7 @@
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
     </row>
-    <row r="6" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
@@ -838,7 +838,7 @@
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>27</v>
       </c>
@@ -858,7 +858,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>32</v>
       </c>
@@ -878,7 +878,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>37</v>
       </c>
@@ -901,7 +901,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>39</v>
       </c>
@@ -924,7 +924,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>41</v>
       </c>
@@ -944,7 +944,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>57</v>
       </c>
@@ -967,7 +967,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
@@ -987,7 +987,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>65</v>
       </c>
@@ -1010,36 +1010,36 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="9"/>
       <c r="F17" s="8"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F33" s="8"/>
     </row>
   </sheetData>
@@ -1071,12 +1071,12 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>43</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
upload sensor board Robin + BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\Documents\GitHub\cosy_cafeteria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16E35E1-F580-462B-A6B1-ABD7EDDFD549}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC3C975-E8FF-4753-9033-BAEF3F72A9DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="100">
   <si>
     <t>Part No.</t>
   </si>
@@ -233,14 +233,114 @@
   </si>
   <si>
     <t>Unbuffered inverter interrupt CCS811</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Murata-Electronics/GRM188C80J106MEA6D?qs=sGAEpiMZZMs0AnBnWHyRQN7%2FAA2D2lPPHKNFzVW0UbJeWppMSPj27Q%3D%3D</t>
+  </si>
+  <si>
+    <t>GRM188C80J106MEA6D</t>
+  </si>
+  <si>
+    <t>10 µF</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Murata-Electronics/GRM188C71A475KE21D?qs=sGAEpiMZZMs0AnBnWHyRQCZFsEygxoaDUfTwU11CgLoHay4CQrnjdQ%3D%3D</t>
+  </si>
+  <si>
+    <t>GRM188C71A475KE21D</t>
+  </si>
+  <si>
+    <t>4,7 µF</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Murata-Electronics/GRM188C71E225KE11J?qs=sGAEpiMZZMs0AnBnWHyRQN7%2FAA2D2lPPoIBVQxy4%252BIYlGUALURHHzw%3D%3D</t>
+  </si>
+  <si>
+    <t>GRM188C71E225KE11J</t>
+  </si>
+  <si>
+    <t>2,2 µF</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Murata-Electronics/GRM188R61C105KA12D?qs=sGAEpiMZZMs0AnBnWHyRQOK8EV8n4V50ILtJpoKun1k%3D</t>
+  </si>
+  <si>
+    <t>GRM188R61C105KA12D</t>
+  </si>
+  <si>
+    <t>1 µF</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Murata-Electronics/GCJ188R71C104MA01D?qs=sGAEpiMZZMs0AnBnWHyRQID2xuQsFd1GofHLF%2FZjZNHccNCeYysMBg%3D%3D</t>
+  </si>
+  <si>
+    <t>GCJ188R71C104MA01D</t>
+  </si>
+  <si>
+    <t>100 nF</t>
+  </si>
+  <si>
+    <t>Capacitors (sensorboards)</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Vishay-Dale/CRCW060322R0FKEAC?qs=sGAEpiMZZMtlubZbdhIBIIZe04wfiaJWhp35UV2eBC0%3D</t>
+  </si>
+  <si>
+    <t>CRCW060322R0FKEAC</t>
+  </si>
+  <si>
+    <t>22 Ohm</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Vishay-Dale/CRCW06034K70FKEAC?qs=sGAEpiMZZMtlubZbdhIBIIZe04wfiaJWtK1b03yAW%2Fw%3D</t>
+  </si>
+  <si>
+    <t>CRCW06034K70FKEAC</t>
+  </si>
+  <si>
+    <t>4,7 kOhm</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Vishay-Dale/CRCW060310K0FKEAC?qs=sGAEpiMZZMtlubZbdhIBIIZe04wfiaJWNE%252B7tlPkrYc%3D</t>
+  </si>
+  <si>
+    <t>CRCW060310K0FKEAC</t>
+  </si>
+  <si>
+    <t>10 kOhm</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Vishay-Dale/CRCW0603100KFKEAC?qs=sGAEpiMZZMtlubZbdhIBIIZe04wfiaJWGPWKSQhf9Xo%3D</t>
+  </si>
+  <si>
+    <t>CRCW0603100KFKEAC</t>
+  </si>
+  <si>
+    <t>100 kOhm</t>
+  </si>
+  <si>
+    <t>Resistors (sensorboard)</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Murata-Electronics/NCU18WF104D60RB?qs=sGAEpiMZZMuBd0%252BwiCVS21gZfQ6Dyzsfx0RadtHN9DipnknzDvt5hw%3D%3D</t>
+  </si>
+  <si>
+    <t>NCU18WF104D60RB</t>
+  </si>
+  <si>
+    <t>100kOhm thermistor</t>
+  </si>
+  <si>
+    <t>Thermistor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -315,7 +415,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -347,6 +447,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -628,15 +731,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S33"/>
+  <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" style="4" customWidth="1"/>
+    <col min="1" max="1" width="25" style="4" customWidth="1"/>
     <col min="2" max="2" width="29" style="4" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" style="4" customWidth="1"/>
@@ -1010,37 +1113,238 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="9"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F26" s="8"/>
-    </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="13">
+        <v>603</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="13">
+        <v>603</v>
+      </c>
+      <c r="E16" s="4">
+        <v>4</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="13">
+        <v>603</v>
+      </c>
+      <c r="E17" s="4">
+        <v>4</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="13">
+        <v>603</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1</v>
+      </c>
+      <c r="F18" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="13">
+        <v>603</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1</v>
+      </c>
+      <c r="F19" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="13">
+        <v>603</v>
+      </c>
+      <c r="E20" s="4">
+        <v>2</v>
+      </c>
+      <c r="F20" s="8">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="13">
+        <v>603</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1</v>
+      </c>
+      <c r="F21" s="8">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="13">
+        <v>603</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+      <c r="F22" s="8">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="13">
+        <v>603</v>
+      </c>
+      <c r="E23" s="4">
+        <v>1</v>
+      </c>
+      <c r="F23" s="8">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="13">
+        <v>603</v>
+      </c>
+      <c r="E24" s="4">
+        <v>1</v>
+      </c>
+      <c r="F24" s="8">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F32" s="8"/>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F33" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -1056,10 +1360,20 @@
     <hyperlink ref="G10" r:id="rId9" xr:uid="{6E401E59-3667-4D7F-ABA4-4D7A0A7A91E1}"/>
     <hyperlink ref="G11" r:id="rId10" xr:uid="{340F4965-1516-4699-A1F1-2E724698C5D3}"/>
     <hyperlink ref="G9" r:id="rId11" xr:uid="{25D5091F-FD09-4C85-B205-63FAF399144A}"/>
-    <hyperlink ref="G14" r:id="rId12" xr:uid="{6FDB2882-2DC7-4B94-A021-37B62FAE5A13}"/>
+    <hyperlink ref="G14" r:id="rId12" xr:uid="{F219828F-DA9F-4E24-8885-ACE67E5D7648}"/>
+    <hyperlink ref="G15" r:id="rId13" xr:uid="{619FAF2D-4D67-4EF0-A7C5-7144F7E3EAE6}"/>
+    <hyperlink ref="G24" r:id="rId14" xr:uid="{19433BBE-7CA5-476E-9B14-87D71C31356D}"/>
+    <hyperlink ref="G23" r:id="rId15" xr:uid="{F4CAC6C2-2D40-434D-9AFB-4DDE36A8C87C}"/>
+    <hyperlink ref="G22" r:id="rId16" xr:uid="{937922AF-B81B-48F4-9080-A991E096793D}"/>
+    <hyperlink ref="G21" r:id="rId17" xr:uid="{994AEB4C-8F58-4FD1-8B14-A388CCC0D84F}"/>
+    <hyperlink ref="G20" r:id="rId18" xr:uid="{76862BDC-620D-4495-88DB-B177298EB46D}"/>
+    <hyperlink ref="G19" r:id="rId19" xr:uid="{AF54CE00-F5E0-4725-9250-4B07912386A7}"/>
+    <hyperlink ref="G18" r:id="rId20" xr:uid="{D0204A60-DF50-404B-BDE0-D959CCB8CCC5}"/>
+    <hyperlink ref="G17" r:id="rId21" xr:uid="{F102EEBB-1B89-4663-9DFD-695FE62BDDA4}"/>
+    <hyperlink ref="G16" r:id="rId22" xr:uid="{0F178DA9-7F2B-48F1-A9A6-17CCAFAF0767}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId23"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Discrete componenten rond IC's en IC's zelfs nagegaan. + toevoeging BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\Documents\GitHub\cosy_cafeteria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC3C975-E8FF-4753-9033-BAEF3F72A9DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6141A891-0D52-4552-BCB9-E7428BC8C3AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="106">
   <si>
     <t>Part No.</t>
   </si>
@@ -46,18 +46,9 @@
     <t xml:space="preserve">Wi-Fi module: </t>
   </si>
   <si>
-    <t>ESP8266-12F</t>
-  </si>
-  <si>
-    <t>https://www.reichelt.com/be/nl/experimenteerbord-esp8266-wifi-module-soldeerbaar-debo-esp8266-12f-p236022.html?PROVID=2788&amp;gclid=Cj0KCQiAkePyBRCEARIsAMy5ScvmAirQ8pxChEbhD-GjxyLzJZJQGJLF0x2Qt61VVOFmUcsClNiI1HMaApqXEALw_wcB&amp;&amp;r=1</t>
-  </si>
-  <si>
     <t>link</t>
   </si>
   <si>
-    <t xml:space="preserve"> DEBO ESP8266-12F</t>
-  </si>
-  <si>
     <t>Battery</t>
   </si>
   <si>
@@ -332,6 +323,33 @@
   </si>
   <si>
     <t>Thermistor</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Wurth-Elektronik/629105150521?qs=%2Fha2pyFaduh5MOEvnTSnzofz1gK6pgHNEIWC6KJrVhsjkEhnkRDmqQ%3D%3D</t>
+  </si>
+  <si>
+    <t>Micro USB  B</t>
+  </si>
+  <si>
+    <t>Wurth 629105150521</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Texas-Instruments/TPS22919DCKT?qs=sGAEpiMZZMuCmTIBzycWfM%252Bsgev%252BoE7sEE2DNGJ1zRc0ZmFhbfdKZg%3D%3D</t>
+  </si>
+  <si>
+    <t>Load switch</t>
+  </si>
+  <si>
+    <t>TPS22919DCKT</t>
+  </si>
+  <si>
+    <t>ESP32</t>
+  </si>
+  <si>
+    <t>ESP32-SOLO-1</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Espressif-Systems/ESP32-SOLO-1?qs=sGAEpiMZZMu3sxpa5v1qrgLFJPTQ7Q2r5D3n3xma6%252Bw%3D</t>
   </si>
 </sst>
 </file>
@@ -731,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S32"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,16 +778,16 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -786,13 +804,13 @@
     </row>
     <row r="2" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4">
@@ -802,7 +820,7 @@
         <v>4.95</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -824,7 +842,7 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="4"/>
@@ -842,13 +860,13 @@
     </row>
     <row r="4" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4">
@@ -858,7 +876,7 @@
         <v>2.17</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -875,16 +893,16 @@
     </row>
     <row r="5" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E5" s="4">
         <v>1</v>
@@ -893,7 +911,7 @@
         <v>1.99</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -911,13 +929,13 @@
     <row r="6" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E6" s="4">
         <v>1</v>
@@ -926,7 +944,7 @@
         <v>0.6</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -943,13 +961,13 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E7" s="4">
         <v>1</v>
@@ -958,18 +976,18 @@
         <v>0.54</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E8" s="4">
         <v>1</v>
@@ -978,276 +996,267 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>38</v>
+      <c r="A9" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
       </c>
       <c r="F9" s="8">
-        <v>6.26</v>
+        <v>1.89</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>40</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="E10" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F10" s="8">
-        <v>10.17</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>44</v>
+        <v>0.38</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+      <c r="F11" s="8">
+        <v>6.26</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="F12" s="8">
+        <v>10.17</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="4">
-        <v>1</v>
-      </c>
-      <c r="F11" s="8">
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="8">
         <v>27.04</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="4">
-        <v>1</v>
-      </c>
-      <c r="F12" s="8">
-        <v>0.35099999999999998</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="4">
-        <v>1</v>
-      </c>
-      <c r="F13" s="8">
-        <v>5.34</v>
-      </c>
       <c r="G13" s="7" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E14" s="4">
         <v>1</v>
       </c>
       <c r="F14" s="8">
-        <v>0.42</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>99</v>
+        <v>3</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D15" s="13">
-        <v>603</v>
+        <v>104</v>
       </c>
       <c r="E15" s="4">
         <v>1</v>
       </c>
       <c r="F15" s="8">
-        <v>0.29699999999999999</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>96</v>
+        <v>3.06</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.42</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D16" s="13">
-        <v>603</v>
-      </c>
-      <c r="E16" s="4">
-        <v>4</v>
-      </c>
-      <c r="F16" s="8">
-        <v>0.09</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D17" s="13">
         <v>603</v>
       </c>
       <c r="E17" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F17" s="8">
-        <v>0.13500000000000001</v>
+        <v>0.29699999999999999</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="B18" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>87</v>
+        <v>91</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>90</v>
       </c>
       <c r="D18" s="13">
         <v>603</v>
       </c>
       <c r="E18" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F18" s="8">
         <v>0.09</v>
       </c>
-      <c r="G18" s="7" t="s">
-        <v>86</v>
+      <c r="G18" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D19" s="13">
         <v>603</v>
       </c>
       <c r="E19" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F19" s="8">
-        <v>0.09</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>82</v>
-      </c>
       <c r="B20" s="4" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D20" s="13">
         <v>603</v>
       </c>
       <c r="E20" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" s="8">
-        <v>0.17100000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D21" s="13">
         <v>603</v>
@@ -1256,38 +1265,41 @@
         <v>1</v>
       </c>
       <c r="F21" s="8">
-        <v>0.14399999999999999</v>
+        <v>0.09</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="B22" s="4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D22" s="13">
         <v>603</v>
       </c>
       <c r="E22" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F22" s="8">
-        <v>0.27900000000000003</v>
+        <v>0.17100000000000001</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D23" s="13">
         <v>603</v>
@@ -1296,18 +1308,18 @@
         <v>1</v>
       </c>
       <c r="F23" s="8">
-        <v>0.28999999999999998</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D24" s="13">
         <v>603</v>
@@ -1316,23 +1328,57 @@
         <v>1</v>
       </c>
       <c r="F24" s="8">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="13">
+        <v>603</v>
+      </c>
+      <c r="E25" s="4">
+        <v>1</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="13">
+        <v>603</v>
+      </c>
+      <c r="E26" s="4">
+        <v>1</v>
+      </c>
+      <c r="F26" s="8">
         <v>0.17100000000000001</v>
       </c>
-      <c r="G24" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F25" s="4"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F26" s="4"/>
+      <c r="G26" s="7" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F27" s="8"/>
+      <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F28" s="8"/>
+      <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F29" s="8"/>
@@ -1345,35 +1391,43 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F32" s="8"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G13" r:id="rId1" xr:uid="{8B37AF3C-3179-401B-9F44-E094BA43E056}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{BE201204-4D76-4D99-A136-97852DAF4D35}"/>
-    <hyperlink ref="G6" r:id="rId3" xr:uid="{C67E4CED-6F3A-4EC3-A9D8-987FB4B57235}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{581F1366-C05C-44C0-8730-D2774468FBE7}"/>
-    <hyperlink ref="G7" r:id="rId5" xr:uid="{AFCDD530-6064-45FD-891D-CCEADAF8BFA1}"/>
-    <hyperlink ref="G8" r:id="rId6" xr:uid="{96DFE09D-FE4D-4147-A8CE-602A5DDFBFA7}"/>
-    <hyperlink ref="G4" r:id="rId7" xr:uid="{682E6110-B477-43CD-9147-49CEB11861DF}"/>
-    <hyperlink ref="G12" r:id="rId8" xr:uid="{426BD05D-D8EF-43D7-A582-AC4F8E600E5F}"/>
-    <hyperlink ref="G10" r:id="rId9" xr:uid="{6E401E59-3667-4D7F-ABA4-4D7A0A7A91E1}"/>
-    <hyperlink ref="G11" r:id="rId10" xr:uid="{340F4965-1516-4699-A1F1-2E724698C5D3}"/>
-    <hyperlink ref="G9" r:id="rId11" xr:uid="{25D5091F-FD09-4C85-B205-63FAF399144A}"/>
-    <hyperlink ref="G14" r:id="rId12" xr:uid="{F219828F-DA9F-4E24-8885-ACE67E5D7648}"/>
-    <hyperlink ref="G15" r:id="rId13" xr:uid="{619FAF2D-4D67-4EF0-A7C5-7144F7E3EAE6}"/>
-    <hyperlink ref="G24" r:id="rId14" xr:uid="{19433BBE-7CA5-476E-9B14-87D71C31356D}"/>
-    <hyperlink ref="G23" r:id="rId15" xr:uid="{F4CAC6C2-2D40-434D-9AFB-4DDE36A8C87C}"/>
-    <hyperlink ref="G22" r:id="rId16" xr:uid="{937922AF-B81B-48F4-9080-A991E096793D}"/>
-    <hyperlink ref="G21" r:id="rId17" xr:uid="{994AEB4C-8F58-4FD1-8B14-A388CCC0D84F}"/>
-    <hyperlink ref="G20" r:id="rId18" xr:uid="{76862BDC-620D-4495-88DB-B177298EB46D}"/>
-    <hyperlink ref="G19" r:id="rId19" xr:uid="{AF54CE00-F5E0-4725-9250-4B07912386A7}"/>
-    <hyperlink ref="G18" r:id="rId20" xr:uid="{D0204A60-DF50-404B-BDE0-D959CCB8CCC5}"/>
-    <hyperlink ref="G17" r:id="rId21" xr:uid="{F102EEBB-1B89-4663-9DFD-695FE62BDDA4}"/>
-    <hyperlink ref="G16" r:id="rId22" xr:uid="{0F178DA9-7F2B-48F1-A9A6-17CCAFAF0767}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{BE201204-4D76-4D99-A136-97852DAF4D35}"/>
+    <hyperlink ref="G6" r:id="rId2" xr:uid="{C67E4CED-6F3A-4EC3-A9D8-987FB4B57235}"/>
+    <hyperlink ref="G5" r:id="rId3" xr:uid="{581F1366-C05C-44C0-8730-D2774468FBE7}"/>
+    <hyperlink ref="G7" r:id="rId4" xr:uid="{AFCDD530-6064-45FD-891D-CCEADAF8BFA1}"/>
+    <hyperlink ref="G8" r:id="rId5" xr:uid="{96DFE09D-FE4D-4147-A8CE-602A5DDFBFA7}"/>
+    <hyperlink ref="G4" r:id="rId6" xr:uid="{682E6110-B477-43CD-9147-49CEB11861DF}"/>
+    <hyperlink ref="G14" r:id="rId7" xr:uid="{426BD05D-D8EF-43D7-A582-AC4F8E600E5F}"/>
+    <hyperlink ref="G12" r:id="rId8" xr:uid="{6E401E59-3667-4D7F-ABA4-4D7A0A7A91E1}"/>
+    <hyperlink ref="G13" r:id="rId9" xr:uid="{340F4965-1516-4699-A1F1-2E724698C5D3}"/>
+    <hyperlink ref="G11" r:id="rId10" xr:uid="{25D5091F-FD09-4C85-B205-63FAF399144A}"/>
+    <hyperlink ref="G16" r:id="rId11" xr:uid="{F219828F-DA9F-4E24-8885-ACE67E5D7648}"/>
+    <hyperlink ref="G17" r:id="rId12" xr:uid="{619FAF2D-4D67-4EF0-A7C5-7144F7E3EAE6}"/>
+    <hyperlink ref="G26" r:id="rId13" xr:uid="{19433BBE-7CA5-476E-9B14-87D71C31356D}"/>
+    <hyperlink ref="G25" r:id="rId14" xr:uid="{F4CAC6C2-2D40-434D-9AFB-4DDE36A8C87C}"/>
+    <hyperlink ref="G24" r:id="rId15" xr:uid="{937922AF-B81B-48F4-9080-A991E096793D}"/>
+    <hyperlink ref="G23" r:id="rId16" xr:uid="{994AEB4C-8F58-4FD1-8B14-A388CCC0D84F}"/>
+    <hyperlink ref="G22" r:id="rId17" xr:uid="{76862BDC-620D-4495-88DB-B177298EB46D}"/>
+    <hyperlink ref="G21" r:id="rId18" xr:uid="{AF54CE00-F5E0-4725-9250-4B07912386A7}"/>
+    <hyperlink ref="G20" r:id="rId19" xr:uid="{D0204A60-DF50-404B-BDE0-D959CCB8CCC5}"/>
+    <hyperlink ref="G19" r:id="rId20" xr:uid="{F102EEBB-1B89-4663-9DFD-695FE62BDDA4}"/>
+    <hyperlink ref="G18" r:id="rId21" xr:uid="{0F178DA9-7F2B-48F1-A9A6-17CCAFAF0767}"/>
+    <hyperlink ref="G9" r:id="rId22" xr:uid="{092811F2-67AA-404B-8561-69F45A6D17C5}"/>
+    <hyperlink ref="G10" r:id="rId23" xr:uid="{3571AC2A-4926-4978-B4A5-820DFE11B665}"/>
+    <hyperlink ref="G15" r:id="rId24" xr:uid="{B06C8493-D698-4F00-8F96-2AB46E697A6F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId23"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId25"/>
 </worksheet>
 </file>
 
@@ -1392,42 +1446,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="4">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="4">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E1" s="8">
         <v>0.70199999999999996</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E2" s="8">
         <v>0.70199999999999996</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added buttons to bom
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\Documents\GitHub\cosy_cafeteria\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthur\Documents\GitHub\cosy_cafeteria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6141A891-0D52-4552-BCB9-E7428BC8C3AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04ED721C-5C27-4B6A-8141-10BC2C33E77B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="555" yWindow="360" windowWidth="20865" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="108">
   <si>
     <t>Part No.</t>
   </si>
@@ -350,17 +350,24 @@
   </si>
   <si>
     <t>https://www.mouser.be/ProductDetail/Espressif-Systems/ESP32-SOLO-1?qs=sGAEpiMZZMu3sxpa5v1qrgLFJPTQ7Q2r5D3n3xma6%252Bw%3D</t>
+  </si>
+  <si>
+    <t>Buttons</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Wurth-Elektronik/430481035816?qs=sGAEpiMZZMuw1rG4%252BG7fptAxWvFrW%2F8uUpLA1Va5WKA%3D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -402,6 +409,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Inherit"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -429,11 +448,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -468,10 +488,17 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Valuta" xfId="2" builtinId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -751,11 +778,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25" style="4" customWidth="1"/>
     <col min="2" max="2" width="29" style="4" customWidth="1"/>
@@ -767,7 +794,7 @@
     <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -802,7 +829,7 @@
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
     </row>
-    <row r="2" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -835,7 +862,7 @@
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
     </row>
-    <row r="3" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -858,7 +885,7 @@
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
     </row>
-    <row r="4" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -891,7 +918,7 @@
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
     </row>
-    <row r="5" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -926,7 +953,7 @@
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
     </row>
-    <row r="6" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
         <v>7</v>
@@ -959,7 +986,7 @@
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="B7" s="4" t="s">
         <v>24</v>
       </c>
@@ -979,7 +1006,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="B8" s="4" t="s">
         <v>29</v>
       </c>
@@ -999,7 +1026,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9" s="4" t="s">
         <v>98</v>
       </c>
@@ -1016,7 +1043,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19">
       <c r="A10" s="4" t="s">
         <v>101</v>
       </c>
@@ -1033,7 +1060,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19">
       <c r="A11" s="11" t="s">
         <v>34</v>
       </c>
@@ -1056,7 +1083,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19">
       <c r="A12" s="11" t="s">
         <v>36</v>
       </c>
@@ -1079,7 +1106,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19">
       <c r="A13" s="11" t="s">
         <v>38</v>
       </c>
@@ -1099,7 +1126,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19">
       <c r="A14" s="4" t="s">
         <v>54</v>
       </c>
@@ -1122,7 +1149,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19">
       <c r="A15" s="4" t="s">
         <v>3</v>
       </c>
@@ -1142,7 +1169,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="A16" s="4" t="s">
         <v>62</v>
       </c>
@@ -1165,7 +1192,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="4" t="s">
         <v>96</v>
       </c>
@@ -1188,7 +1215,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="4" t="s">
         <v>92</v>
       </c>
@@ -1211,7 +1238,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="B19" s="4" t="s">
         <v>88</v>
       </c>
@@ -1231,7 +1258,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="B20" s="4" t="s">
         <v>85</v>
       </c>
@@ -1251,7 +1278,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="B21" s="4" t="s">
         <v>82</v>
       </c>
@@ -1271,7 +1298,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="4" t="s">
         <v>79</v>
       </c>
@@ -1294,7 +1321,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="B23" s="4" t="s">
         <v>75</v>
       </c>
@@ -1314,7 +1341,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="B24" s="4" t="s">
         <v>72</v>
       </c>
@@ -1334,7 +1361,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="B25" s="4" t="s">
         <v>69</v>
       </c>
@@ -1354,7 +1381,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="B26" s="4" t="s">
         <v>66</v>
       </c>
@@ -1374,28 +1401,42 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F28" s="4"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
+      <c r="A28" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" s="15">
+        <v>430481035816</v>
+      </c>
+      <c r="E28" s="4">
+        <v>2</v>
+      </c>
+      <c r="F28" s="14">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:6">
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:6">
       <c r="F34" s="8"/>
     </row>
   </sheetData>
@@ -1425,9 +1466,10 @@
     <hyperlink ref="G9" r:id="rId22" xr:uid="{092811F2-67AA-404B-8561-69F45A6D17C5}"/>
     <hyperlink ref="G10" r:id="rId23" xr:uid="{3571AC2A-4926-4978-B4A5-820DFE11B665}"/>
     <hyperlink ref="G15" r:id="rId24" xr:uid="{B06C8493-D698-4F00-8F96-2AB46E697A6F}"/>
+    <hyperlink ref="G28" r:id="rId25" xr:uid="{B022C6F2-66BF-4E7D-AE9A-E110C3B9196E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId25"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId26"/>
 </worksheet>
 </file>
 
@@ -1439,12 +1481,12 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="11" t="s">
         <v>40</v>
       </c>
@@ -1464,7 +1506,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
Main PCB volledig uitgerust met foorprints voor discrete componenten + BOM aangevuld met alles
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthur\Documents\GitHub\cosy_cafeteria\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\Documents\GitHub\cosy_cafeteria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04ED721C-5C27-4B6A-8141-10BC2C33E77B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84711F6C-84C5-4B39-8B36-CC78FA2CEEDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="555" yWindow="360" windowWidth="20865" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="145">
   <si>
     <t>Part No.</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Function</t>
   </si>
   <si>
-    <t xml:space="preserve">Wi-Fi module: </t>
-  </si>
-  <si>
     <t>link</t>
   </si>
   <si>
@@ -356,18 +353,131 @@
   </si>
   <si>
     <t>https://www.mouser.be/ProductDetail/Wurth-Elektronik/430481035816?qs=sGAEpiMZZMuw1rG4%252BG7fptAxWvFrW%2F8uUpLA1Va5WKA%3D</t>
+  </si>
+  <si>
+    <t>Reverse polarity protection</t>
+  </si>
+  <si>
+    <t>PMOS</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/ON-Semiconductor/NTR2101PT1G?qs=sGAEpiMZZMtqO%252BWUGLBzeMZnYjT0HBB3</t>
+  </si>
+  <si>
+    <t>NTR2101PT1G</t>
+  </si>
+  <si>
+    <t>SOT-23-3</t>
+  </si>
+  <si>
+    <t>Microcontroller + WiFi module</t>
+  </si>
+  <si>
+    <t>Resistors (main board)</t>
+  </si>
+  <si>
+    <t>Blue led</t>
+  </si>
+  <si>
+    <t>Green led</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Vishay-Semiconductors/TLHG44K1L2?qs=sGAEpiMZZMtmwHDZQCdlqWqy6w5Qk3042Twx0LlNbEs%3D</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Vishay-Semiconductors/TLHB44K2M1?qs=%2Fha2pyFaduiIotRAFNomeqo6UScwDzx00yrfnYgvc7A0DrHFviEeOw%3D%3D</t>
+  </si>
+  <si>
+    <t>1,1k</t>
+  </si>
+  <si>
+    <t>47k</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>1,5k</t>
+  </si>
+  <si>
+    <t>2,2k</t>
+  </si>
+  <si>
+    <t>5 Meg</t>
+  </si>
+  <si>
+    <t>Capacitors (main board)</t>
+  </si>
+  <si>
+    <t>Pol Capacitors (main board)</t>
+  </si>
+  <si>
+    <t>5x5,4mm</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/KEMET/EDK476M016A9DAA?qs=sGAEpiMZZMsh%252B1woXyUXj2c%252B1a6x2cYHc9bj3jC8i6I%3D</t>
+  </si>
+  <si>
+    <t>47u/16V</t>
+  </si>
+  <si>
+    <t>EDK476M016A9DAA</t>
+  </si>
+  <si>
+    <t>10u/16V</t>
+  </si>
+  <si>
+    <t>EDH106M016A9BAA</t>
+  </si>
+  <si>
+    <t>4x5,4mm</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/KEMET/EDH106M016A9BAA?qs=sGAEpiMZZMsh%252B1woXyUXjw4z48UYk683%2FsFQSscnRy4%3D</t>
+  </si>
+  <si>
+    <t>3,3u/16V</t>
+  </si>
+  <si>
+    <t>4x5,5mm</t>
+  </si>
+  <si>
+    <t>710-865250340001</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Wurth-Elektronik/865250340001?qs=sGAEpiMZZMsh%252B1woXyUXj4jKQI6sNRw6y8MSDDW21Ks%3D</t>
+  </si>
+  <si>
+    <t>47u/10V X5R</t>
+  </si>
+  <si>
+    <t>GRM31CR61A476ME15L</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Murata-Electronics/GRM31CR61A476ME15L?qs=sGAEpiMZZMs0AnBnWHyRQEM2qvC6XUvUCXMjG942%252BY0%3D</t>
+  </si>
+  <si>
+    <t>1u</t>
+  </si>
+  <si>
+    <t>4,7u</t>
+  </si>
+  <si>
+    <t>0,1u</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="44" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="0000"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,18 +519,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Inherit"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -448,12 +546,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -488,17 +585,13 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
-    <cellStyle name="Valuta" xfId="2" builtinId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -776,13 +869,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S34"/>
+  <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" style="4" customWidth="1"/>
     <col min="2" max="2" width="29" style="4" customWidth="1"/>
@@ -794,7 +887,7 @@
     <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1">
+    <row r="1" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -805,16 +898,16 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -829,15 +922,15 @@
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
     </row>
-    <row r="2" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4">
@@ -847,7 +940,7 @@
         <v>4.95</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -862,14 +955,14 @@
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
     </row>
-    <row r="3" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="3" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="4"/>
@@ -885,15 +978,15 @@
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
     </row>
-    <row r="4" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="4" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="C4" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4">
@@ -903,7 +996,7 @@
         <v>2.17</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -918,18 +1011,18 @@
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
     </row>
-    <row r="5" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="5" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="E5" s="4">
         <v>1</v>
@@ -938,7 +1031,7 @@
         <v>1.99</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -953,16 +1046,16 @@
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
     </row>
-    <row r="6" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="6" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="4">
         <v>1</v>
@@ -971,7 +1064,7 @@
         <v>0.6</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -986,15 +1079,15 @@
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="4">
         <v>1</v>
@@ -1003,18 +1096,18 @@
         <v>0.54</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="4">
         <v>1</v>
@@ -1023,15 +1116,15 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
@@ -1040,404 +1133,661 @@
         <v>1.89</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.33</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="E11" s="4">
+        <v>3</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.38</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="F12" s="8">
+        <v>6.26</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="8">
+        <v>10.17</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="8">
+        <v>27.04</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E10" s="4">
-        <v>3</v>
-      </c>
-      <c r="F10" s="8">
-        <v>0.38</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19">
-      <c r="A11" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="C16" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1</v>
+      </c>
+      <c r="F16" s="8">
+        <v>3.06</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="14">
+        <v>430481035816</v>
+      </c>
+      <c r="E17" s="4">
+        <v>2</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="4">
-        <v>1</v>
-      </c>
-      <c r="F11" s="8">
-        <v>6.26</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19">
-      <c r="A12" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="4">
-        <v>1</v>
-      </c>
-      <c r="F12" s="8">
-        <v>10.17</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="A13" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="4">
-        <v>1</v>
-      </c>
-      <c r="F13" s="8">
-        <v>27.04</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19">
-      <c r="A14" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="4">
-        <v>1</v>
-      </c>
-      <c r="F14" s="8">
-        <v>0.35099999999999998</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="A15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E15" s="4">
-        <v>1</v>
-      </c>
-      <c r="F15" s="8">
-        <v>3.06</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19">
-      <c r="A16" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E18" s="4">
+        <v>1</v>
+      </c>
+      <c r="F18" s="8">
+        <v>0.42</v>
+      </c>
+      <c r="G18" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="4">
-        <v>1</v>
-      </c>
-      <c r="F16" s="8">
-        <v>0.42</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B17" s="4" t="s">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D17" s="13">
-        <v>603</v>
-      </c>
-      <c r="E17" s="4">
-        <v>1</v>
-      </c>
-      <c r="F17" s="8">
-        <v>0.29699999999999999</v>
-      </c>
-      <c r="G17" s="7" t="s">
+      <c r="C19" s="4" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D18" s="13">
-        <v>603</v>
-      </c>
-      <c r="E18" s="4">
-        <v>4</v>
-      </c>
-      <c r="F18" s="8">
-        <v>0.09</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="B19" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="D19" s="13">
         <v>603</v>
       </c>
       <c r="E19" s="4">
+        <v>1</v>
+      </c>
+      <c r="F19" s="8">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+      <c r="F20" s="8">
+        <v>0.92</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1</v>
+      </c>
+      <c r="F21" s="8">
+        <v>0.52</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="4">
+        <v>330</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1206</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="4">
+        <v>680</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1206</v>
+      </c>
+      <c r="E23" s="4">
         <v>4</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1206</v>
+      </c>
+      <c r="E24" s="4">
+        <v>1</v>
+      </c>
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1206</v>
+      </c>
+      <c r="E25" s="4">
+        <v>2</v>
+      </c>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1206</v>
+      </c>
+      <c r="E26" s="4">
+        <v>1</v>
+      </c>
+      <c r="F26" s="8"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D27" s="4">
+        <v>1206</v>
+      </c>
+      <c r="E27" s="4">
+        <v>2</v>
+      </c>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28" s="4">
+        <v>1206</v>
+      </c>
+      <c r="E28" s="4">
+        <v>1</v>
+      </c>
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D29" s="4">
+        <v>1206</v>
+      </c>
+      <c r="E29" s="4">
+        <v>2</v>
+      </c>
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E30" s="4">
+        <v>2</v>
+      </c>
+      <c r="F30" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E31" s="4">
+        <v>4</v>
+      </c>
+      <c r="F31" s="8">
+        <v>0.22</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E32" s="4">
+        <v>3</v>
+      </c>
+      <c r="F32" s="8">
+        <v>0.24</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D33" s="4">
+        <v>1206</v>
+      </c>
+      <c r="E33" s="4">
+        <v>1</v>
+      </c>
+      <c r="F33" s="8">
+        <v>0.76</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D34" s="4">
+        <v>1206</v>
+      </c>
+      <c r="E34" s="4">
+        <v>3</v>
+      </c>
+      <c r="F34" s="8"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D35" s="4">
+        <v>1206</v>
+      </c>
+      <c r="E35" s="4">
+        <v>4</v>
+      </c>
+      <c r="F35" s="8"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D36" s="4">
+        <v>1206</v>
+      </c>
+      <c r="E36" s="4">
+        <v>2</v>
+      </c>
+      <c r="F36" s="8"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" s="13">
+        <v>603</v>
+      </c>
+      <c r="E37" s="4">
+        <v>4</v>
+      </c>
+      <c r="F37" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" s="13">
+        <v>603</v>
+      </c>
+      <c r="E38" s="4">
+        <v>4</v>
+      </c>
+      <c r="F38" s="8">
         <v>0.13500000000000001</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="B20" s="4" t="s">
+      <c r="G38" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C20" s="4" t="s">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="13">
+      <c r="C39" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" s="13">
         <v>603</v>
       </c>
-      <c r="E20" s="4">
-        <v>1</v>
-      </c>
-      <c r="F20" s="8">
+      <c r="E39" s="4">
+        <v>1</v>
+      </c>
+      <c r="F39" s="8">
         <v>0.09</v>
       </c>
-      <c r="G20" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="B21" s="4" t="s">
+      <c r="G39" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="4" t="s">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D21" s="13">
+      <c r="C40" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40" s="13">
         <v>603</v>
       </c>
-      <c r="E21" s="4">
-        <v>1</v>
-      </c>
-      <c r="F21" s="8">
+      <c r="E40" s="4">
+        <v>1</v>
+      </c>
+      <c r="F40" s="8">
         <v>0.09</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="4" t="s">
+      <c r="G40" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B22" s="4" t="s">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="13">
+      <c r="C41" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" s="13">
         <v>603</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E41" s="4">
         <v>2</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F41" s="8">
         <v>0.17100000000000001</v>
       </c>
-      <c r="G22" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="B23" s="4" t="s">
+      <c r="G41" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="4" t="s">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="13">
+      <c r="C42" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D42" s="13">
         <v>603</v>
       </c>
-      <c r="E23" s="4">
-        <v>1</v>
-      </c>
-      <c r="F23" s="8">
+      <c r="E42" s="4">
+        <v>1</v>
+      </c>
+      <c r="F42" s="8">
         <v>0.14399999999999999</v>
       </c>
-      <c r="G23" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="B24" s="4" t="s">
+      <c r="G42" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="4" t="s">
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="13">
+      <c r="C43" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43" s="13">
         <v>603</v>
       </c>
-      <c r="E24" s="4">
-        <v>1</v>
-      </c>
-      <c r="F24" s="8">
+      <c r="E43" s="4">
+        <v>1</v>
+      </c>
+      <c r="F43" s="8">
         <v>0.27900000000000003</v>
       </c>
-      <c r="G24" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="B25" s="4" t="s">
+      <c r="G43" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="4" t="s">
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="13">
+      <c r="C44" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44" s="13">
         <v>603</v>
       </c>
-      <c r="E25" s="4">
-        <v>1</v>
-      </c>
-      <c r="F25" s="8">
+      <c r="E44" s="4">
+        <v>1</v>
+      </c>
+      <c r="F44" s="8">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G25" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="B26" s="4" t="s">
+      <c r="G44" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="4" t="s">
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="13">
+      <c r="C45" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" s="13">
         <v>603</v>
       </c>
-      <c r="E26" s="4">
-        <v>1</v>
-      </c>
-      <c r="F26" s="8">
+      <c r="E45" s="4">
+        <v>1</v>
+      </c>
+      <c r="F45" s="8">
         <v>0.17100000000000001</v>
       </c>
-      <c r="G26" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="F27" s="4"/>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C28" s="15">
-        <v>430481035816</v>
-      </c>
-      <c r="E28" s="4">
-        <v>2</v>
-      </c>
-      <c r="F28" s="14">
-        <v>0.45900000000000002</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="F29" s="8"/>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="F30" s="8"/>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="F31" s="8"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="F32" s="8"/>
-    </row>
-    <row r="33" spans="6:6">
-      <c r="F33" s="8"/>
-    </row>
-    <row r="34" spans="6:6">
-      <c r="F34" s="8"/>
+      <c r="G45" s="7" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -1448,28 +1798,35 @@
     <hyperlink ref="G7" r:id="rId4" xr:uid="{AFCDD530-6064-45FD-891D-CCEADAF8BFA1}"/>
     <hyperlink ref="G8" r:id="rId5" xr:uid="{96DFE09D-FE4D-4147-A8CE-602A5DDFBFA7}"/>
     <hyperlink ref="G4" r:id="rId6" xr:uid="{682E6110-B477-43CD-9147-49CEB11861DF}"/>
-    <hyperlink ref="G14" r:id="rId7" xr:uid="{426BD05D-D8EF-43D7-A582-AC4F8E600E5F}"/>
-    <hyperlink ref="G12" r:id="rId8" xr:uid="{6E401E59-3667-4D7F-ABA4-4D7A0A7A91E1}"/>
-    <hyperlink ref="G13" r:id="rId9" xr:uid="{340F4965-1516-4699-A1F1-2E724698C5D3}"/>
-    <hyperlink ref="G11" r:id="rId10" xr:uid="{25D5091F-FD09-4C85-B205-63FAF399144A}"/>
-    <hyperlink ref="G16" r:id="rId11" xr:uid="{F219828F-DA9F-4E24-8885-ACE67E5D7648}"/>
-    <hyperlink ref="G17" r:id="rId12" xr:uid="{619FAF2D-4D67-4EF0-A7C5-7144F7E3EAE6}"/>
-    <hyperlink ref="G26" r:id="rId13" xr:uid="{19433BBE-7CA5-476E-9B14-87D71C31356D}"/>
-    <hyperlink ref="G25" r:id="rId14" xr:uid="{F4CAC6C2-2D40-434D-9AFB-4DDE36A8C87C}"/>
-    <hyperlink ref="G24" r:id="rId15" xr:uid="{937922AF-B81B-48F4-9080-A991E096793D}"/>
-    <hyperlink ref="G23" r:id="rId16" xr:uid="{994AEB4C-8F58-4FD1-8B14-A388CCC0D84F}"/>
-    <hyperlink ref="G22" r:id="rId17" xr:uid="{76862BDC-620D-4495-88DB-B177298EB46D}"/>
-    <hyperlink ref="G21" r:id="rId18" xr:uid="{AF54CE00-F5E0-4725-9250-4B07912386A7}"/>
-    <hyperlink ref="G20" r:id="rId19" xr:uid="{D0204A60-DF50-404B-BDE0-D959CCB8CCC5}"/>
-    <hyperlink ref="G19" r:id="rId20" xr:uid="{F102EEBB-1B89-4663-9DFD-695FE62BDDA4}"/>
-    <hyperlink ref="G18" r:id="rId21" xr:uid="{0F178DA9-7F2B-48F1-A9A6-17CCAFAF0767}"/>
+    <hyperlink ref="G15" r:id="rId7" xr:uid="{426BD05D-D8EF-43D7-A582-AC4F8E600E5F}"/>
+    <hyperlink ref="G13" r:id="rId8" xr:uid="{6E401E59-3667-4D7F-ABA4-4D7A0A7A91E1}"/>
+    <hyperlink ref="G14" r:id="rId9" xr:uid="{340F4965-1516-4699-A1F1-2E724698C5D3}"/>
+    <hyperlink ref="G12" r:id="rId10" xr:uid="{25D5091F-FD09-4C85-B205-63FAF399144A}"/>
+    <hyperlink ref="G18" r:id="rId11" xr:uid="{F219828F-DA9F-4E24-8885-ACE67E5D7648}"/>
+    <hyperlink ref="G19" r:id="rId12" xr:uid="{619FAF2D-4D67-4EF0-A7C5-7144F7E3EAE6}"/>
+    <hyperlink ref="G45" r:id="rId13" xr:uid="{19433BBE-7CA5-476E-9B14-87D71C31356D}"/>
+    <hyperlink ref="G44" r:id="rId14" xr:uid="{F4CAC6C2-2D40-434D-9AFB-4DDE36A8C87C}"/>
+    <hyperlink ref="G43" r:id="rId15" xr:uid="{937922AF-B81B-48F4-9080-A991E096793D}"/>
+    <hyperlink ref="G42" r:id="rId16" xr:uid="{994AEB4C-8F58-4FD1-8B14-A388CCC0D84F}"/>
+    <hyperlink ref="G41" r:id="rId17" xr:uid="{76862BDC-620D-4495-88DB-B177298EB46D}"/>
+    <hyperlink ref="G40" r:id="rId18" xr:uid="{AF54CE00-F5E0-4725-9250-4B07912386A7}"/>
+    <hyperlink ref="G39" r:id="rId19" xr:uid="{D0204A60-DF50-404B-BDE0-D959CCB8CCC5}"/>
+    <hyperlink ref="G38" r:id="rId20" xr:uid="{F102EEBB-1B89-4663-9DFD-695FE62BDDA4}"/>
+    <hyperlink ref="G37" r:id="rId21" xr:uid="{0F178DA9-7F2B-48F1-A9A6-17CCAFAF0767}"/>
     <hyperlink ref="G9" r:id="rId22" xr:uid="{092811F2-67AA-404B-8561-69F45A6D17C5}"/>
-    <hyperlink ref="G10" r:id="rId23" xr:uid="{3571AC2A-4926-4978-B4A5-820DFE11B665}"/>
-    <hyperlink ref="G15" r:id="rId24" xr:uid="{B06C8493-D698-4F00-8F96-2AB46E697A6F}"/>
-    <hyperlink ref="G28" r:id="rId25" xr:uid="{B022C6F2-66BF-4E7D-AE9A-E110C3B9196E}"/>
+    <hyperlink ref="G11" r:id="rId23" xr:uid="{3571AC2A-4926-4978-B4A5-820DFE11B665}"/>
+    <hyperlink ref="G16" r:id="rId24" xr:uid="{B06C8493-D698-4F00-8F96-2AB46E697A6F}"/>
+    <hyperlink ref="G17" r:id="rId25" xr:uid="{B022C6F2-66BF-4E7D-AE9A-E110C3B9196E}"/>
+    <hyperlink ref="G10" r:id="rId26" xr:uid="{5D93DF65-24C6-4E51-A510-3921BED8E11B}"/>
+    <hyperlink ref="G21" r:id="rId27" xr:uid="{189818F7-AA8F-4727-9185-CEA50EF2695D}"/>
+    <hyperlink ref="G20" r:id="rId28" xr:uid="{53AA5B85-A885-4355-9507-7D4FAD9E6E7A}"/>
+    <hyperlink ref="G30" r:id="rId29" xr:uid="{258B17CA-7BC0-49B1-9646-4348361BA522}"/>
+    <hyperlink ref="G31" r:id="rId30" xr:uid="{850A7ECD-14D3-4AE8-9F8D-82209F865128}"/>
+    <hyperlink ref="G32" r:id="rId31" xr:uid="{15EB3110-02A8-4DE6-85CA-C6ADD5F5B2B7}"/>
+    <hyperlink ref="G33" r:id="rId32" xr:uid="{4098B0A1-B48A-4B0E-B2AA-660FD27291C7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId26"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId33"/>
 </worksheet>
 </file>
 
@@ -1481,49 +1838,49 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="4">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="8">
         <v>0.70199999999999996</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>50</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>51</v>
-      </c>
-      <c r="D2" t="s">
-        <v>52</v>
       </c>
       <c r="E2" s="8">
         <v>0.70199999999999996</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Eerste plaatsing van componenten op PCB
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\Documents\GitHub\cosy_cafeteria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84711F6C-84C5-4B39-8B36-CC78FA2CEEDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8579323-84EA-4045-AF36-DFD87ABEF628}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -871,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:G45"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Bom update package 0603 => 1206 sensor board
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\Documents\GitHub\cosy_cafeteria\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gebruikersnaam\Documents\GitHub\cosy_cafeteria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8579323-84EA-4045-AF36-DFD87ABEF628}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0151CB-82B3-426E-AFE2-05FBF14CEB04}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -223,48 +223,18 @@
     <t>Unbuffered inverter interrupt CCS811</t>
   </si>
   <si>
-    <t>https://www.mouser.be/ProductDetail/Murata-Electronics/GRM188C80J106MEA6D?qs=sGAEpiMZZMs0AnBnWHyRQN7%2FAA2D2lPPHKNFzVW0UbJeWppMSPj27Q%3D%3D</t>
-  </si>
-  <si>
-    <t>GRM188C80J106MEA6D</t>
-  </si>
-  <si>
     <t>10 µF</t>
   </si>
   <si>
-    <t>https://www.mouser.be/ProductDetail/Murata-Electronics/GRM188C71A475KE21D?qs=sGAEpiMZZMs0AnBnWHyRQCZFsEygxoaDUfTwU11CgLoHay4CQrnjdQ%3D%3D</t>
-  </si>
-  <si>
-    <t>GRM188C71A475KE21D</t>
-  </si>
-  <si>
     <t>4,7 µF</t>
   </si>
   <si>
-    <t>https://www.mouser.be/ProductDetail/Murata-Electronics/GRM188C71E225KE11J?qs=sGAEpiMZZMs0AnBnWHyRQN7%2FAA2D2lPPoIBVQxy4%252BIYlGUALURHHzw%3D%3D</t>
-  </si>
-  <si>
-    <t>GRM188C71E225KE11J</t>
-  </si>
-  <si>
     <t>2,2 µF</t>
   </si>
   <si>
-    <t>https://www.mouser.be/ProductDetail/Murata-Electronics/GRM188R61C105KA12D?qs=sGAEpiMZZMs0AnBnWHyRQOK8EV8n4V50ILtJpoKun1k%3D</t>
-  </si>
-  <si>
-    <t>GRM188R61C105KA12D</t>
-  </si>
-  <si>
     <t>1 µF</t>
   </si>
   <si>
-    <t>https://www.mouser.be/ProductDetail/Murata-Electronics/GCJ188R71C104MA01D?qs=sGAEpiMZZMs0AnBnWHyRQID2xuQsFd1GofHLF%2FZjZNHccNCeYysMBg%3D%3D</t>
-  </si>
-  <si>
-    <t>GCJ188R71C104MA01D</t>
-  </si>
-  <si>
     <t>100 nF</t>
   </si>
   <si>
@@ -274,36 +244,18 @@
     <t>https://www.mouser.be/ProductDetail/Vishay-Dale/CRCW060322R0FKEAC?qs=sGAEpiMZZMtlubZbdhIBIIZe04wfiaJWhp35UV2eBC0%3D</t>
   </si>
   <si>
-    <t>CRCW060322R0FKEAC</t>
-  </si>
-  <si>
     <t>22 Ohm</t>
   </si>
   <si>
     <t>https://www.mouser.be/ProductDetail/Vishay-Dale/CRCW06034K70FKEAC?qs=sGAEpiMZZMtlubZbdhIBIIZe04wfiaJWtK1b03yAW%2Fw%3D</t>
   </si>
   <si>
-    <t>CRCW06034K70FKEAC</t>
-  </si>
-  <si>
     <t>4,7 kOhm</t>
   </si>
   <si>
-    <t>https://www.mouser.be/ProductDetail/Vishay-Dale/CRCW060310K0FKEAC?qs=sGAEpiMZZMtlubZbdhIBIIZe04wfiaJWNE%252B7tlPkrYc%3D</t>
-  </si>
-  <si>
-    <t>CRCW060310K0FKEAC</t>
-  </si>
-  <si>
     <t>10 kOhm</t>
   </si>
   <si>
-    <t>https://www.mouser.be/ProductDetail/Vishay-Dale/CRCW0603100KFKEAC?qs=sGAEpiMZZMtlubZbdhIBIIZe04wfiaJWGPWKSQhf9Xo%3D</t>
-  </si>
-  <si>
-    <t>CRCW0603100KFKEAC</t>
-  </si>
-  <si>
     <t>100 kOhm</t>
   </si>
   <si>
@@ -467,6 +419,54 @@
   </si>
   <si>
     <t>0,1u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRCW1206100KFKEAC </t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Vishay-Dale/CRCW1206100KFKEAC?qs=%2Fha2pyFaduhVH%2Fy0xAAQ%252BgElv4ycej%2FOIqR%2FeWpwuzpdhLgmwM29sdKv0jEvr3JO</t>
+  </si>
+  <si>
+    <t>CRCW120610K0FKEAC</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Vishay-Dale/CRCW120610K0FKEAC?qs=%2Fha2pyFaduhVH%2Fy0xAAQ%252BlD6lCjlTDfxo%2FeDNnf1Mf8Mr6SzFIO6us8PB0tWM7HL</t>
+  </si>
+  <si>
+    <t>CRCW12064K70FKEAC</t>
+  </si>
+  <si>
+    <t>CRCW120622R0FKEAC</t>
+  </si>
+  <si>
+    <t>GRM319R72A104KA01D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Murata-Electronics/GRM319R72A104KA01D?qs=sGAEpiMZZMs0AnBnWHyRQLChrxA3Kg%252BjKBAXgBSnp7s%3D</t>
+  </si>
+  <si>
+    <t>GRM31MR71C105KA01L</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Murata-Electronics/GRM31MR71C105KA01L?qs=sGAEpiMZZMs0AnBnWHyRQFvwHJRtJOIYKi8VPJ919ZA%3D</t>
+  </si>
+  <si>
+    <t>GRM31MR71C225KA35L</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Murata-Electronics/GRM31MR71C225KA35L?qs=sGAEpiMZZMs0AnBnWHyRQCxUk0Tc%252BSyhEDLjoZeRG%252BU%3D</t>
+  </si>
+  <si>
+    <t>GRM31CR61A475KA01L</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Murata-Electronics/GRM31CR61A475KA01L?qs=sGAEpiMZZMs0AnBnWHyRQLSmaItDK%2Fu45dji7X%252Bwi6Y%3D</t>
+  </si>
+  <si>
+    <t>GRM319C81C106MA12J</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Murata-Electronics/GRM319C81C106MA12J?qs=sGAEpiMZZMs0AnBnWHyRQAsAWwhBCY7b9qntZx9zSmKH4l%252BxP1cciQ%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -871,23 +871,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="G29" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" style="4" customWidth="1"/>
     <col min="2" max="2" width="29" style="4" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="220.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="3" max="3" width="18.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="220.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -922,7 +922,7 @@
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
     </row>
-    <row r="2" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -955,7 +955,7 @@
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
     </row>
-    <row r="3" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -978,7 +978,7 @@
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
     </row>
-    <row r="4" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1011,7 +1011,7 @@
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
     </row>
-    <row r="5" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
@@ -1046,7 +1046,7 @@
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
     </row>
-    <row r="6" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
         <v>6</v>
@@ -1079,7 +1079,7 @@
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>23</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>28</v>
       </c>
@@ -1119,12 +1119,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
@@ -1133,21 +1133,21 @@
         <v>1.89</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="E10" s="4">
         <v>1</v>
@@ -1156,15 +1156,15 @@
         <v>0.33</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="E11" s="4">
         <v>3</v>
@@ -1173,10 +1173,10 @@
         <v>0.38</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>33</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>35</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>37</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>53</v>
       </c>
@@ -1265,15 +1265,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="E16" s="4">
         <v>1</v>
@@ -1282,12 +1282,12 @@
         <v>3.06</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C17" s="14">
         <v>430481035816</v>
@@ -1299,10 +1299,10 @@
         <v>0.45900000000000002</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>61</v>
       </c>
@@ -1325,15 +1325,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="D19" s="13">
         <v>603</v>
@@ -1345,15 +1345,15 @@
         <v>0.29699999999999999</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="E20" s="4">
         <v>1</v>
@@ -1362,15 +1362,15 @@
         <v>0.92</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="E21" s="4">
         <v>1</v>
@@ -1379,12 +1379,12 @@
         <v>0.52</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="B22" s="4">
         <v>330</v>
@@ -1397,7 +1397,7 @@
       </c>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B23" s="4">
         <v>680</v>
       </c>
@@ -1409,9 +1409,9 @@
       </c>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B24" s="4" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="D24" s="4">
         <v>1206</v>
@@ -1421,9 +1421,9 @@
       </c>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="D25" s="4">
         <v>1206</v>
@@ -1433,9 +1433,9 @@
       </c>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B26" s="4" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="D26" s="4">
         <v>1206</v>
@@ -1445,9 +1445,9 @@
       </c>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B27" s="4" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="D27" s="4">
         <v>1206</v>
@@ -1457,9 +1457,9 @@
       </c>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B28" s="4" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="D28" s="4">
         <v>1206</v>
@@ -1469,9 +1469,9 @@
       </c>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="D29" s="4">
         <v>1206</v>
@@ -1481,18 +1481,18 @@
       </c>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="E30" s="4">
         <v>2</v>
@@ -1501,18 +1501,18 @@
         <v>0.23</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B31" s="4" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="E31" s="4">
         <v>4</v>
@@ -1521,18 +1521,18 @@
         <v>0.22</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="E32" s="4">
         <v>3</v>
@@ -1541,18 +1541,18 @@
         <v>0.24</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="D33" s="4">
         <v>1206</v>
@@ -1564,12 +1564,12 @@
         <v>0.76</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B34" s="4" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="D34" s="4">
         <v>1206</v>
@@ -1579,9 +1579,9 @@
       </c>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B35" s="4" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="D35" s="4">
         <v>1206</v>
@@ -1591,9 +1591,9 @@
       </c>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B36" s="4" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="D36" s="4">
         <v>1206</v>
@@ -1603,18 +1603,18 @@
       </c>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="D37" s="13">
-        <v>603</v>
+        <v>1206</v>
       </c>
       <c r="E37" s="4">
         <v>4</v>
@@ -1623,38 +1623,38 @@
         <v>0.09</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B38" s="4" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
       <c r="D38" s="13">
-        <v>603</v>
+        <v>1206</v>
       </c>
       <c r="E38" s="4">
         <v>4</v>
       </c>
       <c r="F38" s="8">
-        <v>0.13500000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B39" s="4" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>83</v>
+        <v>133</v>
       </c>
       <c r="D39" s="13">
-        <v>603</v>
+        <v>1206</v>
       </c>
       <c r="E39" s="4">
         <v>1</v>
@@ -1663,18 +1663,18 @@
         <v>0.09</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B40" s="4" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>80</v>
+        <v>134</v>
       </c>
       <c r="D40" s="13">
-        <v>603</v>
+        <v>1206</v>
       </c>
       <c r="E40" s="4">
         <v>1</v>
@@ -1683,110 +1683,110 @@
         <v>0.09</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>76</v>
+        <v>135</v>
       </c>
       <c r="D41" s="13">
-        <v>603</v>
+        <v>1206</v>
       </c>
       <c r="E41" s="4">
         <v>2</v>
       </c>
       <c r="F41" s="8">
-        <v>0.17100000000000001</v>
+        <v>0.35</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B42" s="4" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>73</v>
+        <v>137</v>
       </c>
       <c r="D42" s="13">
-        <v>603</v>
+        <v>1206</v>
       </c>
       <c r="E42" s="4">
         <v>1</v>
       </c>
       <c r="F42" s="8">
-        <v>0.14399999999999999</v>
+        <v>0.26100000000000001</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B43" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>70</v>
+        <v>139</v>
       </c>
       <c r="D43" s="13">
-        <v>603</v>
+        <v>1206</v>
       </c>
       <c r="E43" s="4">
         <v>1</v>
       </c>
       <c r="F43" s="8">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B44" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D44" s="13">
+        <v>1206</v>
+      </c>
+      <c r="E44" s="4">
+        <v>1</v>
+      </c>
+      <c r="F44" s="8">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B45" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D45" s="13">
+        <v>1206</v>
+      </c>
+      <c r="E45" s="4">
+        <v>1</v>
+      </c>
+      <c r="F45" s="8">
         <v>0.27900000000000003</v>
       </c>
-      <c r="G43" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D44" s="13">
-        <v>603</v>
-      </c>
-      <c r="E44" s="4">
-        <v>1</v>
-      </c>
-      <c r="F44" s="8">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D45" s="13">
-        <v>603</v>
-      </c>
-      <c r="E45" s="4">
-        <v>1</v>
-      </c>
-      <c r="F45" s="8">
-        <v>0.17100000000000001</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>63</v>
+      <c r="G45" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1804,29 +1804,24 @@
     <hyperlink ref="G12" r:id="rId10" xr:uid="{25D5091F-FD09-4C85-B205-63FAF399144A}"/>
     <hyperlink ref="G18" r:id="rId11" xr:uid="{F219828F-DA9F-4E24-8885-ACE67E5D7648}"/>
     <hyperlink ref="G19" r:id="rId12" xr:uid="{619FAF2D-4D67-4EF0-A7C5-7144F7E3EAE6}"/>
-    <hyperlink ref="G45" r:id="rId13" xr:uid="{19433BBE-7CA5-476E-9B14-87D71C31356D}"/>
-    <hyperlink ref="G44" r:id="rId14" xr:uid="{F4CAC6C2-2D40-434D-9AFB-4DDE36A8C87C}"/>
-    <hyperlink ref="G43" r:id="rId15" xr:uid="{937922AF-B81B-48F4-9080-A991E096793D}"/>
-    <hyperlink ref="G42" r:id="rId16" xr:uid="{994AEB4C-8F58-4FD1-8B14-A388CCC0D84F}"/>
-    <hyperlink ref="G41" r:id="rId17" xr:uid="{76862BDC-620D-4495-88DB-B177298EB46D}"/>
-    <hyperlink ref="G40" r:id="rId18" xr:uid="{AF54CE00-F5E0-4725-9250-4B07912386A7}"/>
-    <hyperlink ref="G39" r:id="rId19" xr:uid="{D0204A60-DF50-404B-BDE0-D959CCB8CCC5}"/>
-    <hyperlink ref="G38" r:id="rId20" xr:uid="{F102EEBB-1B89-4663-9DFD-695FE62BDDA4}"/>
-    <hyperlink ref="G37" r:id="rId21" xr:uid="{0F178DA9-7F2B-48F1-A9A6-17CCAFAF0767}"/>
-    <hyperlink ref="G9" r:id="rId22" xr:uid="{092811F2-67AA-404B-8561-69F45A6D17C5}"/>
-    <hyperlink ref="G11" r:id="rId23" xr:uid="{3571AC2A-4926-4978-B4A5-820DFE11B665}"/>
-    <hyperlink ref="G16" r:id="rId24" xr:uid="{B06C8493-D698-4F00-8F96-2AB46E697A6F}"/>
-    <hyperlink ref="G17" r:id="rId25" xr:uid="{B022C6F2-66BF-4E7D-AE9A-E110C3B9196E}"/>
-    <hyperlink ref="G10" r:id="rId26" xr:uid="{5D93DF65-24C6-4E51-A510-3921BED8E11B}"/>
-    <hyperlink ref="G21" r:id="rId27" xr:uid="{189818F7-AA8F-4727-9185-CEA50EF2695D}"/>
-    <hyperlink ref="G20" r:id="rId28" xr:uid="{53AA5B85-A885-4355-9507-7D4FAD9E6E7A}"/>
-    <hyperlink ref="G30" r:id="rId29" xr:uid="{258B17CA-7BC0-49B1-9646-4348361BA522}"/>
-    <hyperlink ref="G31" r:id="rId30" xr:uid="{850A7ECD-14D3-4AE8-9F8D-82209F865128}"/>
-    <hyperlink ref="G32" r:id="rId31" xr:uid="{15EB3110-02A8-4DE6-85CA-C6ADD5F5B2B7}"/>
-    <hyperlink ref="G33" r:id="rId32" xr:uid="{4098B0A1-B48A-4B0E-B2AA-660FD27291C7}"/>
+    <hyperlink ref="G44" r:id="rId13" xr:uid="{F4CAC6C2-2D40-434D-9AFB-4DDE36A8C87C}"/>
+    <hyperlink ref="G40" r:id="rId14" xr:uid="{AF54CE00-F5E0-4725-9250-4B07912386A7}"/>
+    <hyperlink ref="G39" r:id="rId15" xr:uid="{D0204A60-DF50-404B-BDE0-D959CCB8CCC5}"/>
+    <hyperlink ref="G37" r:id="rId16" xr:uid="{0F178DA9-7F2B-48F1-A9A6-17CCAFAF0767}"/>
+    <hyperlink ref="G9" r:id="rId17" xr:uid="{092811F2-67AA-404B-8561-69F45A6D17C5}"/>
+    <hyperlink ref="G11" r:id="rId18" xr:uid="{3571AC2A-4926-4978-B4A5-820DFE11B665}"/>
+    <hyperlink ref="G16" r:id="rId19" xr:uid="{B06C8493-D698-4F00-8F96-2AB46E697A6F}"/>
+    <hyperlink ref="G17" r:id="rId20" xr:uid="{B022C6F2-66BF-4E7D-AE9A-E110C3B9196E}"/>
+    <hyperlink ref="G10" r:id="rId21" xr:uid="{5D93DF65-24C6-4E51-A510-3921BED8E11B}"/>
+    <hyperlink ref="G21" r:id="rId22" xr:uid="{189818F7-AA8F-4727-9185-CEA50EF2695D}"/>
+    <hyperlink ref="G20" r:id="rId23" xr:uid="{53AA5B85-A885-4355-9507-7D4FAD9E6E7A}"/>
+    <hyperlink ref="G30" r:id="rId24" xr:uid="{258B17CA-7BC0-49B1-9646-4348361BA522}"/>
+    <hyperlink ref="G31" r:id="rId25" xr:uid="{850A7ECD-14D3-4AE8-9F8D-82209F865128}"/>
+    <hyperlink ref="G32" r:id="rId26" xr:uid="{15EB3110-02A8-4DE6-85CA-C6ADD5F5B2B7}"/>
+    <hyperlink ref="G33" r:id="rId27" xr:uid="{4098B0A1-B48A-4B0E-B2AA-660FD27291C7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId33"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId28"/>
 </worksheet>
 </file>
 
@@ -1838,12 +1833,12 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>39</v>
       </c>
@@ -1863,7 +1858,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
Eerste pcb layouts ensorboard
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gebruikersnaam\Documents\GitHub\cosy_cafeteria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0151CB-82B3-426E-AFE2-05FBF14CEB04}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C58307-47BA-47DA-AD5F-0269FDFF2F01}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -871,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G29" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1336,7 +1336,7 @@
         <v>77</v>
       </c>
       <c r="D19" s="13">
-        <v>603</v>
+        <v>1608</v>
       </c>
       <c r="E19" s="4">
         <v>1</v>

</xml_diff>

<commit_message>
Finished MainPCB + generated gerber files + aanpassingen BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gebruikersnaam\Documents\GitHub\cosy_cafeteria\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\Documents\GitHub\cosy_cafeteria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C58307-47BA-47DA-AD5F-0269FDFF2F01}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D45EB4-489E-40F2-BA84-076FD0B01A97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="148">
   <si>
     <t>Part No.</t>
   </si>
@@ -238,9 +238,6 @@
     <t>100 nF</t>
   </si>
   <si>
-    <t>Capacitors (sensorboards)</t>
-  </si>
-  <si>
     <t>https://www.mouser.be/ProductDetail/Vishay-Dale/CRCW060322R0FKEAC?qs=sGAEpiMZZMtlubZbdhIBIIZe04wfiaJWhp35UV2eBC0%3D</t>
   </si>
   <si>
@@ -253,15 +250,9 @@
     <t>4,7 kOhm</t>
   </si>
   <si>
-    <t>10 kOhm</t>
-  </si>
-  <si>
     <t>100 kOhm</t>
   </si>
   <si>
-    <t>Resistors (sensorboard)</t>
-  </si>
-  <si>
     <t>https://www.mouser.be/ProductDetail/Murata-Electronics/NCU18WF104D60RB?qs=sGAEpiMZZMuBd0%252BwiCVS21gZfQ6Dyzsfx0RadtHN9DipnknzDvt5hw%3D%3D</t>
   </si>
   <si>
@@ -361,9 +352,6 @@
     <t>5 Meg</t>
   </si>
   <si>
-    <t>Capacitors (main board)</t>
-  </si>
-  <si>
     <t>Pol Capacitors (main board)</t>
   </si>
   <si>
@@ -412,27 +400,12 @@
     <t>https://www.mouser.be/ProductDetail/Murata-Electronics/GRM31CR61A476ME15L?qs=sGAEpiMZZMs0AnBnWHyRQEM2qvC6XUvUCXMjG942%252BY0%3D</t>
   </si>
   <si>
-    <t>1u</t>
-  </si>
-  <si>
-    <t>4,7u</t>
-  </si>
-  <si>
-    <t>0,1u</t>
-  </si>
-  <si>
     <t xml:space="preserve">CRCW1206100KFKEAC </t>
   </si>
   <si>
     <t>https://www.mouser.be/ProductDetail/Vishay-Dale/CRCW1206100KFKEAC?qs=%2Fha2pyFaduhVH%2Fy0xAAQ%252BgElv4ycej%2FOIqR%2FeWpwuzpdhLgmwM29sdKv0jEvr3JO</t>
   </si>
   <si>
-    <t>CRCW120610K0FKEAC</t>
-  </si>
-  <si>
-    <t>https://www.mouser.be/ProductDetail/Vishay-Dale/CRCW120610K0FKEAC?qs=%2Fha2pyFaduhVH%2Fy0xAAQ%252BlD6lCjlTDfxo%2FeDNnf1Mf8Mr6SzFIO6us8PB0tWM7HL</t>
-  </si>
-  <si>
     <t>CRCW12064K70FKEAC</t>
   </si>
   <si>
@@ -467,6 +440,42 @@
   </si>
   <si>
     <t>https://www.mouser.be/ProductDetail/Murata-Electronics/GRM319C81C106MA12J?qs=sGAEpiMZZMs0AnBnWHyRQAsAWwhBCY7b9qntZx9zSmKH4l%252BxP1cciQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Vishay-Dale/CRCW12061K50FKEAC?qs=sGAEpiMZZMtlubZbdhIBIIZe04wfiaJWIl2r2x2TK58%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Vishay-Dale/CRCW120647K0FKEAC?qs=sGAEpiMZZMtlubZbdhIBIIZe04wfiaJWrst357c%252BTkE%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Vishay-Dale/CRCW1206680RJNEAIF?qs=sGAEpiMZZMtlubZbdhIBIE5SSkTEu4Rq1ljP5VEJtpM%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Vishay-Dale/CRCW1206330RFKEA?qs=sGAEpiMZZMu61qfTUdNhGyptJL5EcUtRieka4diDHRQ%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Vishay-Dale/CRCW120610K0FKEAC?qs=sGAEpiMZZMtlubZbdhIBIIZe04wfiaJWFuAq5dn3JRk%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Vishay-Dale/CRCW12062K20FKEAC?qs=sGAEpiMZZMtlubZbdhIBIIZe04wfiaJWTvWqPWcHQI8%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Vishay-Dale/CRCW12061K10FKEA?qs=sGAEpiMZZMtlubZbdhIBIE9Nj%2FZ3XBsuPUS7%252Bm6Pivw%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Vishay-Dale/CRCW12064M99FKEA?qs=sGAEpiMZZMu61qfTUdNhG3XwnH6YDjgjmNIcJbg5HAc%3D</t>
+  </si>
+  <si>
+    <t>Capacitors</t>
+  </si>
+  <si>
+    <t>11 Pin header</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Harwin/M20-9771146?qs=sGAEpiMZZMs%252BGHln7q6pmzlZUuX%2F53qj9Y4EVXUNSN4%3D</t>
+  </si>
+  <si>
+    <t>11 jumper wires female-female</t>
   </si>
 </sst>
 </file>
@@ -869,25 +878,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S45"/>
+  <dimension ref="A1:S43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" style="4" customWidth="1"/>
     <col min="2" max="2" width="29" style="4" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="220.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="4"/>
+    <col min="3" max="3" width="18.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="220.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -922,7 +931,7 @@
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
     </row>
-    <row r="2" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -955,7 +964,7 @@
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
     </row>
-    <row r="3" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -978,7 +987,7 @@
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
     </row>
-    <row r="4" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1011,7 +1020,7 @@
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
     </row>
-    <row r="5" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
@@ -1046,7 +1055,7 @@
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
     </row>
-    <row r="6" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
         <v>6</v>
@@ -1079,7 +1088,7 @@
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>23</v>
       </c>
@@ -1099,7 +1108,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>28</v>
       </c>
@@ -1119,12 +1128,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
@@ -1133,21 +1142,21 @@
         <v>1.89</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>95</v>
       </c>
       <c r="E10" s="4">
         <v>1</v>
@@ -1156,15 +1165,15 @@
         <v>0.33</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E11" s="4">
         <v>3</v>
@@ -1173,10 +1182,10 @@
         <v>0.38</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>33</v>
       </c>
@@ -1199,7 +1208,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>35</v>
       </c>
@@ -1222,7 +1231,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>37</v>
       </c>
@@ -1242,7 +1251,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>53</v>
       </c>
@@ -1265,15 +1274,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E16" s="4">
         <v>1</v>
@@ -1282,12 +1291,12 @@
         <v>3.06</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C17" s="14">
         <v>430481035816</v>
@@ -1299,10 +1308,10 @@
         <v>0.45900000000000002</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>61</v>
       </c>
@@ -1325,15 +1334,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D19" s="13">
         <v>1608</v>
@@ -1345,15 +1354,15 @@
         <v>0.29699999999999999</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="E20" s="4">
         <v>1</v>
@@ -1362,15 +1371,15 @@
         <v>0.92</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E21" s="4">
         <v>1</v>
@@ -1379,299 +1388,344 @@
         <v>0.52</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B22" s="4">
+        <v>145</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="4">
+        <v>2</v>
+      </c>
+      <c r="F22" s="8">
+        <v>0.32</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D24" s="13">
+        <v>1206</v>
+      </c>
+      <c r="E24" s="4">
+        <v>1</v>
+      </c>
+      <c r="F24" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
         <v>330</v>
-      </c>
-      <c r="D22" s="4">
-        <v>1206</v>
-      </c>
-      <c r="E22" s="4">
-        <v>1</v>
-      </c>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="4">
-        <v>680</v>
-      </c>
-      <c r="D23" s="4">
-        <v>1206</v>
-      </c>
-      <c r="E23" s="4">
-        <v>4</v>
-      </c>
-      <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D24" s="4">
-        <v>1206</v>
-      </c>
-      <c r="E24" s="4">
-        <v>1</v>
-      </c>
-      <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="D25" s="4">
         <v>1206</v>
       </c>
       <c r="E25" s="4">
-        <v>2</v>
-      </c>
-      <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="4" t="s">
-        <v>107</v>
+        <v>1</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="4">
+        <v>680</v>
       </c>
       <c r="D26" s="4">
         <v>1206</v>
       </c>
       <c r="E26" s="4">
-        <v>1</v>
-      </c>
-      <c r="F26" s="8"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="F26" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D27" s="4">
         <v>1206</v>
       </c>
       <c r="E27" s="4">
-        <v>2</v>
-      </c>
-      <c r="F27" s="8"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F27" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D28" s="4">
         <v>1206</v>
       </c>
       <c r="E28" s="4">
-        <v>1</v>
-      </c>
-      <c r="F28" s="8"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="F28" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D29" s="4">
         <v>1206</v>
       </c>
       <c r="E29" s="4">
-        <v>2</v>
-      </c>
-      <c r="F29" s="8"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>110</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F29" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
-        <v>113</v>
+        <v>71</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>111</v>
+        <v>124</v>
+      </c>
+      <c r="D30" s="13">
+        <v>1206</v>
       </c>
       <c r="E30" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" s="8">
-        <v>0.23</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.09</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>117</v>
+        <v>102</v>
+      </c>
+      <c r="D31" s="4">
+        <v>1206</v>
       </c>
       <c r="E31" s="4">
+        <v>6</v>
+      </c>
+      <c r="F31" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" s="4">
+        <v>1206</v>
+      </c>
+      <c r="E32" s="4">
+        <v>1</v>
+      </c>
+      <c r="F32" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" s="13">
+        <v>1206</v>
+      </c>
+      <c r="E33" s="4">
         <v>4</v>
       </c>
-      <c r="F31" s="8">
-        <v>0.22</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B32" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E32" s="4">
-        <v>3</v>
-      </c>
-      <c r="F32" s="8">
-        <v>0.24</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B33" s="4" t="s">
+      <c r="F33" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D33" s="4">
-        <v>1206</v>
-      </c>
-      <c r="E33" s="4">
-        <v>1</v>
-      </c>
-      <c r="F33" s="8">
-        <v>0.76</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="D34" s="4">
         <v>1206</v>
       </c>
       <c r="E34" s="4">
+        <v>2</v>
+      </c>
+      <c r="F34" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" s="4">
+        <v>2</v>
+      </c>
+      <c r="F35" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E36" s="4">
+        <v>4</v>
+      </c>
+      <c r="F36" s="8">
+        <v>0.22</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E37" s="4">
         <v>3</v>
       </c>
-      <c r="F34" s="8"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="4" t="s">
+      <c r="F37" s="8">
+        <v>0.24</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>126</v>
-      </c>
-      <c r="D35" s="4">
-        <v>1206</v>
-      </c>
-      <c r="E35" s="4">
-        <v>4</v>
-      </c>
-      <c r="F35" s="8"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D36" s="4">
-        <v>1206</v>
-      </c>
-      <c r="E36" s="4">
-        <v>2</v>
-      </c>
-      <c r="F36" s="8"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="D37" s="13">
-        <v>1206</v>
-      </c>
-      <c r="E37" s="4">
-        <v>4</v>
-      </c>
-      <c r="F37" s="8">
-        <v>0.09</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B38" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="D38" s="13">
         <v>1206</v>
       </c>
       <c r="E38" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F38" s="8">
-        <v>0.09</v>
+        <v>0.35</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D39" s="13">
         <v>1206</v>
       </c>
       <c r="E39" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F39" s="8">
-        <v>0.09</v>
+        <v>0.26100000000000001</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D40" s="13">
         <v>1206</v>
@@ -1680,41 +1734,38 @@
         <v>1</v>
       </c>
       <c r="F40" s="8">
-        <v>0.09</v>
+        <v>0.29699999999999999</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
-        <v>68</v>
-      </c>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D41" s="13">
         <v>1206</v>
       </c>
       <c r="E41" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F41" s="8">
-        <v>0.35</v>
+        <v>0.36899999999999999</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D42" s="13">
         <v>1206</v>
@@ -1723,70 +1774,30 @@
         <v>1</v>
       </c>
       <c r="F42" s="8">
-        <v>0.26100000000000001</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="D43" s="13">
+        <v>120</v>
+      </c>
+      <c r="D43" s="4">
         <v>1206</v>
       </c>
       <c r="E43" s="4">
         <v>1</v>
       </c>
       <c r="F43" s="8">
-        <v>0.29699999999999999</v>
-      </c>
-      <c r="G43" s="7" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B44" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D44" s="13">
-        <v>1206</v>
-      </c>
-      <c r="E44" s="4">
-        <v>1</v>
-      </c>
-      <c r="F44" s="8">
-        <v>0.36899999999999999</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B45" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D45" s="13">
-        <v>1206</v>
-      </c>
-      <c r="E45" s="4">
-        <v>1</v>
-      </c>
-      <c r="F45" s="8">
-        <v>0.27900000000000003</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>144</v>
+        <v>0.76</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1804,10 +1815,10 @@
     <hyperlink ref="G12" r:id="rId10" xr:uid="{25D5091F-FD09-4C85-B205-63FAF399144A}"/>
     <hyperlink ref="G18" r:id="rId11" xr:uid="{F219828F-DA9F-4E24-8885-ACE67E5D7648}"/>
     <hyperlink ref="G19" r:id="rId12" xr:uid="{619FAF2D-4D67-4EF0-A7C5-7144F7E3EAE6}"/>
-    <hyperlink ref="G44" r:id="rId13" xr:uid="{F4CAC6C2-2D40-434D-9AFB-4DDE36A8C87C}"/>
-    <hyperlink ref="G40" r:id="rId14" xr:uid="{AF54CE00-F5E0-4725-9250-4B07912386A7}"/>
-    <hyperlink ref="G39" r:id="rId15" xr:uid="{D0204A60-DF50-404B-BDE0-D959CCB8CCC5}"/>
-    <hyperlink ref="G37" r:id="rId16" xr:uid="{0F178DA9-7F2B-48F1-A9A6-17CCAFAF0767}"/>
+    <hyperlink ref="G41" r:id="rId13" xr:uid="{F4CAC6C2-2D40-434D-9AFB-4DDE36A8C87C}"/>
+    <hyperlink ref="G24" r:id="rId14" xr:uid="{AF54CE00-F5E0-4725-9250-4B07912386A7}"/>
+    <hyperlink ref="G30" r:id="rId15" xr:uid="{D0204A60-DF50-404B-BDE0-D959CCB8CCC5}"/>
+    <hyperlink ref="G33" r:id="rId16" xr:uid="{0F178DA9-7F2B-48F1-A9A6-17CCAFAF0767}"/>
     <hyperlink ref="G9" r:id="rId17" xr:uid="{092811F2-67AA-404B-8561-69F45A6D17C5}"/>
     <hyperlink ref="G11" r:id="rId18" xr:uid="{3571AC2A-4926-4978-B4A5-820DFE11B665}"/>
     <hyperlink ref="G16" r:id="rId19" xr:uid="{B06C8493-D698-4F00-8F96-2AB46E697A6F}"/>
@@ -1815,13 +1826,23 @@
     <hyperlink ref="G10" r:id="rId21" xr:uid="{5D93DF65-24C6-4E51-A510-3921BED8E11B}"/>
     <hyperlink ref="G21" r:id="rId22" xr:uid="{189818F7-AA8F-4727-9185-CEA50EF2695D}"/>
     <hyperlink ref="G20" r:id="rId23" xr:uid="{53AA5B85-A885-4355-9507-7D4FAD9E6E7A}"/>
-    <hyperlink ref="G30" r:id="rId24" xr:uid="{258B17CA-7BC0-49B1-9646-4348361BA522}"/>
-    <hyperlink ref="G31" r:id="rId25" xr:uid="{850A7ECD-14D3-4AE8-9F8D-82209F865128}"/>
-    <hyperlink ref="G32" r:id="rId26" xr:uid="{15EB3110-02A8-4DE6-85CA-C6ADD5F5B2B7}"/>
-    <hyperlink ref="G33" r:id="rId27" xr:uid="{4098B0A1-B48A-4B0E-B2AA-660FD27291C7}"/>
+    <hyperlink ref="G35" r:id="rId24" xr:uid="{258B17CA-7BC0-49B1-9646-4348361BA522}"/>
+    <hyperlink ref="G36" r:id="rId25" xr:uid="{850A7ECD-14D3-4AE8-9F8D-82209F865128}"/>
+    <hyperlink ref="G37" r:id="rId26" xr:uid="{15EB3110-02A8-4DE6-85CA-C6ADD5F5B2B7}"/>
+    <hyperlink ref="G43" r:id="rId27" xr:uid="{4098B0A1-B48A-4B0E-B2AA-660FD27291C7}"/>
+    <hyperlink ref="G28" r:id="rId28" xr:uid="{927B8ABD-8118-4683-A15B-0391A64D25B0}"/>
+    <hyperlink ref="G32" r:id="rId29" xr:uid="{3D6C7538-7627-4B9D-8B3D-D15061B23A16}"/>
+    <hyperlink ref="G26" r:id="rId30" xr:uid="{279BEC83-2CA6-41EF-9AE3-B022003183BD}"/>
+    <hyperlink ref="G25" r:id="rId31" xr:uid="{B87D843C-6406-4920-A163-0FC7D8E02A21}"/>
+    <hyperlink ref="G31" r:id="rId32" xr:uid="{A6F2E23E-2ECA-4D71-89DA-48017F96F806}"/>
+    <hyperlink ref="G29" r:id="rId33" xr:uid="{3DDD5F0B-8AB4-49FE-94B2-EB4BFC2F6341}"/>
+    <hyperlink ref="G27" r:id="rId34" xr:uid="{5DC8BB42-9D99-4E5B-8243-EDE54EB8887E}"/>
+    <hyperlink ref="G34" r:id="rId35" xr:uid="{32C0F45F-109A-4F6D-A45D-7B21ECE165A6}"/>
+    <hyperlink ref="G39" r:id="rId36" xr:uid="{A9F14920-0F15-4721-A0F0-758F592CC933}"/>
+    <hyperlink ref="G22" r:id="rId37" xr:uid="{2D9C6DEC-9229-4AAB-A2FA-39A71B7475D3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId38"/>
 </worksheet>
 </file>
 
@@ -1833,12 +1854,12 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>39</v>
       </c>
@@ -1858,7 +1879,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>

</xml_diff>